<commit_message>
Updated .gitignore to exclude excel lock files, working on BOM data....counting screws
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77E3FC9-D1DD-44B0-8C79-5632C12BBD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59101659-E853-4FA4-86BC-0B6363FCE5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-40068" yWindow="-4392" windowWidth="34560" windowHeight="19188" activeTab="1" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
@@ -498,24 +498,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -989,7 +989,7 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,27 +1008,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
       <c r="M1" s="24"/>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="38"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -1073,12 +1073,12 @@
       <c r="O2" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="P2" s="33" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="7"/>
@@ -1096,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="L3" s="10"/>
-      <c r="M3" s="34">
+      <c r="M3" s="32">
         <v>6</v>
       </c>
       <c r="N3" s="7"/>
@@ -1104,7 +1104,7 @@
       <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="8">
@@ -1116,10 +1116,10 @@
       <c r="D4" s="23">
         <v>8</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="34">
         <v>6</v>
       </c>
-      <c r="F4" s="38"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="23"/>
       <c r="H4" s="12"/>
       <c r="I4" s="8">
@@ -1138,13 +1138,13 @@
       <c r="N4" s="8">
         <v>2</v>
       </c>
-      <c r="O4" s="38">
+      <c r="O4" s="34">
         <v>3</v>
       </c>
       <c r="P4" s="12"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="30" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="8">
@@ -1159,7 +1159,7 @@
       <c r="E5" s="23">
         <v>32</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="34">
         <v>3</v>
       </c>
       <c r="G5" s="23"/>
@@ -1169,7 +1169,7 @@
       <c r="I5" s="8">
         <v>44</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="34">
         <v>8</v>
       </c>
       <c r="K5" s="23"/>
@@ -1188,7 +1188,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="30" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="8"/>
@@ -1208,7 +1208,7 @@
       <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="8"/>
@@ -1228,7 +1228,7 @@
       <c r="P7" s="12"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="30" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="8"/>
@@ -1248,7 +1248,7 @@
       <c r="P8" s="12"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="4"/>
@@ -1286,31 +1286,31 @@
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10">
-        <f>SUM(G4:G9)</f>
+        <f t="shared" ref="G10:M10" si="0">SUM(G4:G9)</f>
         <v>0</v>
       </c>
       <c r="H10" s="10">
-        <f>SUM(H4:H9)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I10" s="10">
-        <f>SUM(I4:I9)</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="J10" s="10">
-        <f>SUM(J4:J9)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="K10" s="10">
-        <f>SUM(K4:K9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L10" s="10">
-        <f>SUM(L4:L9)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="M10" s="10">
-        <f>SUM(M4:M9)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="N10" s="10"/>
@@ -1485,40 +1485,40 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="e">
-        <f t="shared" ref="D15:M15" si="0">D14*D13</f>
+        <f t="shared" ref="D15:M15" si="1">D14*D13</f>
         <v>#REF!</v>
       </c>
       <c r="E15" s="15" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
       <c r="H15" s="15" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
       <c r="I15" s="15" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
       <c r="J15" s="15" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
       <c r="K15" s="15" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
       <c r="L15" s="15" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
       <c r="M15" s="15" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
       <c r="N15" s="21" t="e">

</xml_diff>

<commit_message>
Updated screw count through joint 3 and started working on the forearm
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59101659-E853-4FA4-86BC-0B6363FCE5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8BACCD-0F7F-49D7-A92B-2D608711D4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40068" yWindow="-4392" windowWidth="34560" windowHeight="19188" activeTab="1" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
+    <workbookView xWindow="-39792" yWindow="-4116" windowWidth="34560" windowHeight="19188" activeTab="1" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Nut</t>
   </si>
@@ -224,6 +224,18 @@
   </si>
   <si>
     <t>8x22x7</t>
+  </si>
+  <si>
+    <t>0?</t>
+  </si>
+  <si>
+    <t>THERE ARE MISSING SCREWS IN THE OVERALL ARM DESIGN!!!!!! IN THE FOREARM, BE SURE TO COUNT THEM</t>
+  </si>
+  <si>
+    <t>THEY ARE AROUND THE MOUNTING ARM/Mounting Plate</t>
+  </si>
+  <si>
+    <t>AND BE VERY CAREFUL TO MAKE SURE THERE ARE NOT ANYMORE</t>
   </si>
 </sst>
 </file>
@@ -258,12 +270,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -448,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -516,6 +540,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -986,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAFB602-290B-4982-B78B-7ABFBEFF08D7}">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,14 +1178,14 @@
       <c r="A5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="39">
         <v>29</v>
       </c>
       <c r="C5" s="23">
         <v>8</v>
       </c>
       <c r="D5" s="23">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E5" s="23">
         <v>32</v>
@@ -1166,7 +1197,7 @@
       <c r="H5" s="12">
         <v>6</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="39">
         <v>44</v>
       </c>
       <c r="J5" s="34">
@@ -1191,41 +1222,85 @@
       <c r="A6" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="8">
+        <v>13</v>
+      </c>
+      <c r="C6" s="23">
+        <v>4</v>
+      </c>
+      <c r="D6" s="34">
+        <v>8</v>
+      </c>
+      <c r="E6" s="34">
+        <v>6</v>
+      </c>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="23"/>
+      <c r="H6" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="8">
+        <v>12</v>
+      </c>
+      <c r="J6" s="34">
+        <v>4</v>
+      </c>
       <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="12"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="L6" s="34">
+        <v>6</v>
+      </c>
+      <c r="M6" s="12">
+        <v>6</v>
+      </c>
+      <c r="N6" s="8">
+        <v>2</v>
+      </c>
+      <c r="O6" s="34">
+        <v>3</v>
+      </c>
+      <c r="P6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="12"/>
+      <c r="B7" s="41">
+        <v>19</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42">
+        <v>4</v>
+      </c>
+      <c r="E7" s="42">
+        <v>6</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="43">
+        <v>6</v>
+      </c>
+      <c r="I7" s="41">
+        <v>12</v>
+      </c>
+      <c r="J7" s="42">
+        <v>4</v>
+      </c>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42">
+        <v>12</v>
+      </c>
+      <c r="M7" s="43"/>
+      <c r="N7" s="41">
+        <v>1</v>
+      </c>
+      <c r="O7" s="42">
+        <v>3</v>
+      </c>
+      <c r="P7" s="43">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
@@ -1236,7 +1311,9 @@
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
+      <c r="G8" s="23">
+        <v>6</v>
+      </c>
       <c r="H8" s="12"/>
       <c r="I8" s="8"/>
       <c r="J8" s="23"/>
@@ -1273,33 +1350,33 @@
       </c>
       <c r="B10" s="10">
         <f>SUM(B4:B9)</f>
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10">
         <f>SUM(D4:D9)</f>
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E10" s="10">
         <f>SUM(E4:E9)</f>
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10">
         <f t="shared" ref="G10:M10" si="0">SUM(G4:G9)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I10" s="10">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="J10" s="10">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="K10" s="10">
         <f t="shared" si="0"/>
@@ -1307,11 +1384,11 @@
       </c>
       <c r="L10" s="10">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="M10" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
@@ -1557,8 +1634,21 @@
       <c r="K21" s="28"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>64</v>
+      </c>
       <c r="N23" s="13"/>
       <c r="P23" s="13"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1566,7 +1656,7 @@
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="N1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:M9 O4">
+  <conditionalFormatting sqref="B4:M9 O4 O6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Hardware section of BOM mostly completed, counting is done, need to double check all highlighted cells, measure finger screws, and collect pricing/links/identifier numbers
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8BACCD-0F7F-49D7-A92B-2D608711D4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EE05AA-E7BF-4BAB-94A4-940B09B1C9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39792" yWindow="-4116" windowWidth="34560" windowHeight="19188" activeTab="1" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
+    <workbookView xWindow="-46188" yWindow="-7152" windowWidth="46296" windowHeight="26136" activeTab="1" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
-    <sheet name="Bolts and Bearing Counter" sheetId="1" r:id="rId2"/>
+    <sheet name="Hardware" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>Nut</t>
   </si>
@@ -202,40 +202,40 @@
     <t>Bearings</t>
   </si>
   <si>
-    <t>75x95x10mm</t>
-  </si>
-  <si>
-    <t>12x28x8mm</t>
-  </si>
-  <si>
     <t>Standoffs</t>
   </si>
   <si>
     <t>Standoff</t>
   </si>
   <si>
-    <t>all joints include the arm they are attached to at the bottom</t>
-  </si>
-  <si>
-    <t>joint 1 has double arms</t>
-  </si>
-  <si>
-    <t>joint 3 has single arm</t>
-  </si>
-  <si>
     <t>8x22x7</t>
   </si>
   <si>
     <t>0?</t>
   </si>
   <si>
-    <t>THERE ARE MISSING SCREWS IN THE OVERALL ARM DESIGN!!!!!! IN THE FOREARM, BE SURE TO COUNT THEM</t>
-  </si>
-  <si>
-    <t>THEY ARE AROUND THE MOUNTING ARM/Mounting Plate</t>
-  </si>
-  <si>
-    <t>AND BE VERY CAREFUL TO MAKE SURE THERE ARE NOT ANYMORE</t>
+    <t>M2.5</t>
+  </si>
+  <si>
+    <t>Belts - 300mm GT2</t>
+  </si>
+  <si>
+    <t>30x37x4</t>
+  </si>
+  <si>
+    <t>WHAT SIZE SCREWS WERE USED TO ATTACH THE FINGERS TO THE CARRIER ADAPTERS? ADD THAT IN</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>12x28x8</t>
+  </si>
+  <si>
+    <t>75x95x10</t>
+  </si>
+  <si>
+    <t>9XXXXXXXX</t>
   </si>
 </sst>
 </file>
@@ -245,7 +245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,8 +269,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,7 +300,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -481,44 +508,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -526,8 +528,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,13 +546,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -569,6 +610,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD33939"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -877,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CD22FD-255E-455F-872D-D755421F4957}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1053,15 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1017,646 +1071,909 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAFB602-290B-4982-B78B-7ABFBEFF08D7}">
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="36" t="s">
+      <c r="O1" s="18"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="37"/>
-      <c r="P1" s="38"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="21"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="27">
+        <v>8</v>
+      </c>
+      <c r="D2" s="28">
+        <v>5</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="30">
+        <v>6</v>
+      </c>
+      <c r="H2" s="30">
+        <v>10</v>
+      </c>
+      <c r="I2" s="30">
+        <v>12</v>
+      </c>
+      <c r="J2" s="30">
+        <v>15</v>
+      </c>
+      <c r="K2" s="30">
+        <v>25</v>
+      </c>
+      <c r="L2" s="30">
+        <v>30</v>
+      </c>
+      <c r="M2" s="30">
+        <v>35</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="30">
+        <v>10</v>
+      </c>
+      <c r="P2" s="30">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="30">
+        <v>45</v>
+      </c>
+      <c r="R2" s="27">
+        <v>60</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="39">
+        <v>17</v>
+      </c>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="13">
+        <v>6</v>
+      </c>
+      <c r="S3" s="39"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="13"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33">
+        <v>13</v>
+      </c>
+      <c r="F4" s="35">
+        <v>4</v>
+      </c>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35">
+        <v>8</v>
+      </c>
+      <c r="J4" s="35">
+        <v>6</v>
+      </c>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="33">
+        <v>12</v>
+      </c>
+      <c r="O4" s="35">
+        <v>4</v>
+      </c>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35">
+        <v>6</v>
+      </c>
+      <c r="R4" s="34">
+        <v>6</v>
+      </c>
+      <c r="S4" s="33">
+        <v>2</v>
+      </c>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35">
+        <v>3</v>
+      </c>
+      <c r="V4" s="34"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="16">
+        <v>29</v>
+      </c>
+      <c r="F5" s="14">
+        <v>8</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14">
+        <v>16</v>
+      </c>
+      <c r="J5" s="14">
+        <v>32</v>
+      </c>
+      <c r="K5" s="14">
+        <v>3</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="24">
+        <v>6</v>
+      </c>
+      <c r="N5" s="16">
+        <v>44</v>
+      </c>
+      <c r="O5" s="14">
+        <v>8</v>
+      </c>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14">
+        <v>24</v>
+      </c>
+      <c r="R5" s="14"/>
+      <c r="S5" s="23">
+        <v>2</v>
+      </c>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14">
+        <v>6</v>
+      </c>
+      <c r="V5" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33">
+        <v>13</v>
+      </c>
+      <c r="F6" s="35">
+        <v>4</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35">
+        <v>8</v>
+      </c>
+      <c r="J6" s="35">
+        <v>6</v>
+      </c>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="3">
+      <c r="N6" s="33">
         <v>12</v>
       </c>
-      <c r="E2" s="3">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="O6" s="35">
+        <v>4</v>
+      </c>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35">
+        <v>6</v>
+      </c>
+      <c r="R6" s="34">
+        <v>6</v>
+      </c>
+      <c r="S6" s="33">
+        <v>2</v>
+      </c>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35">
+        <v>3</v>
+      </c>
+      <c r="V6" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="3">
-        <v>30</v>
-      </c>
-      <c r="H2" s="3">
-        <v>35</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23">
+        <v>19</v>
+      </c>
+      <c r="F7" s="14">
+        <v>4</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14">
+        <v>4</v>
+      </c>
+      <c r="J7" s="14">
+        <v>6</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="24">
+        <v>6</v>
+      </c>
+      <c r="N7" s="23">
+        <v>12</v>
+      </c>
+      <c r="O7" s="14">
+        <v>4</v>
+      </c>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14">
+        <v>12</v>
+      </c>
+      <c r="R7" s="14"/>
+      <c r="S7" s="23">
+        <v>1</v>
+      </c>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14">
+        <v>3</v>
+      </c>
+      <c r="V7" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="33">
+        <v>8</v>
+      </c>
+      <c r="E8" s="33">
+        <v>32</v>
+      </c>
+      <c r="F8" s="35">
+        <v>8</v>
+      </c>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35">
+        <v>16</v>
+      </c>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35">
+        <v>12</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35">
+        <v>14</v>
+      </c>
+      <c r="M8" s="35"/>
+      <c r="N8" s="33">
+        <v>12</v>
+      </c>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35">
         <v>10</v>
       </c>
-      <c r="K2" s="3">
+      <c r="Q8" s="35">
+        <v>2</v>
+      </c>
+      <c r="R8" s="35"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="35">
+        <v>2</v>
+      </c>
+      <c r="U8" s="35"/>
+      <c r="V8" s="34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="36">
+        <v>4</v>
+      </c>
+      <c r="C9" s="37">
+        <v>4</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36">
+        <v>12</v>
+      </c>
+      <c r="F9" s="38">
+        <v>4</v>
+      </c>
+      <c r="G9" s="38">
+        <v>8</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="38">
+        <v>12</v>
+      </c>
+      <c r="K9" s="14"/>
+      <c r="L9" s="38">
+        <v>4</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="37"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="46">
+        <f>SUM(B3:B9)</f>
+        <v>4</v>
+      </c>
+      <c r="C10" s="46">
+        <f t="shared" ref="C10:V10" si="0">SUM(C3:C9)</f>
+        <v>4</v>
+      </c>
+      <c r="D10" s="46">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10" s="46">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="F10" s="46">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="G10" s="46">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H10" s="46">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="L2" s="3">
-        <v>45</v>
-      </c>
-      <c r="M2" s="25">
-        <v>60</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="P2" s="33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="7">
-        <v>17</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10">
-        <v>11</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="32">
-        <v>6</v>
-      </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="11"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="8">
-        <v>13</v>
-      </c>
-      <c r="C4" s="23">
-        <v>4</v>
-      </c>
-      <c r="D4" s="23">
-        <v>8</v>
-      </c>
-      <c r="E4" s="34">
-        <v>6</v>
-      </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="8">
-        <v>12</v>
-      </c>
-      <c r="J4" s="23">
-        <v>4</v>
-      </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23">
-        <v>6</v>
-      </c>
-      <c r="M4" s="12">
-        <v>6</v>
-      </c>
-      <c r="N4" s="8">
-        <v>2</v>
-      </c>
-      <c r="O4" s="34">
+      <c r="I10" s="46">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="J10" s="46">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="K10" s="46">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P4" s="12"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="39">
-        <v>29</v>
-      </c>
-      <c r="C5" s="23">
-        <v>8</v>
-      </c>
-      <c r="D5" s="23">
-        <v>16</v>
-      </c>
-      <c r="E5" s="23">
-        <v>32</v>
-      </c>
-      <c r="F5" s="34">
-        <v>3</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="12">
-        <v>6</v>
-      </c>
-      <c r="I5" s="39">
-        <v>44</v>
-      </c>
-      <c r="J5" s="34">
-        <v>8</v>
-      </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23">
-        <v>24</v>
-      </c>
-      <c r="M5" s="12"/>
-      <c r="N5" s="8">
-        <v>2</v>
-      </c>
-      <c r="O5" s="23">
-        <v>6</v>
-      </c>
-      <c r="P5" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="8">
-        <v>13</v>
-      </c>
-      <c r="C6" s="23">
-        <v>4</v>
-      </c>
-      <c r="D6" s="34">
-        <v>8</v>
-      </c>
-      <c r="E6" s="34">
-        <v>6</v>
-      </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" s="8">
-        <v>12</v>
-      </c>
-      <c r="J6" s="34">
-        <v>4</v>
-      </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="34">
-        <v>6</v>
-      </c>
-      <c r="M6" s="12">
-        <v>6</v>
-      </c>
-      <c r="N6" s="8">
-        <v>2</v>
-      </c>
-      <c r="O6" s="34">
-        <v>3</v>
-      </c>
-      <c r="P6" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="41">
-        <v>19</v>
-      </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42">
-        <v>4</v>
-      </c>
-      <c r="E7" s="42">
-        <v>6</v>
-      </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="43">
-        <v>6</v>
-      </c>
-      <c r="I7" s="41">
-        <v>12</v>
-      </c>
-      <c r="J7" s="42">
-        <v>4</v>
-      </c>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42">
-        <v>12</v>
-      </c>
-      <c r="M7" s="43"/>
-      <c r="N7" s="41">
-        <v>1</v>
-      </c>
-      <c r="O7" s="42">
-        <v>3</v>
-      </c>
-      <c r="P7" s="43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23">
-        <v>6</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="12"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="10">
-        <f>SUM(B4:B9)</f>
-        <v>74</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10">
-        <f>SUM(D4:D9)</f>
-        <v>36</v>
-      </c>
-      <c r="E10" s="10">
-        <f>SUM(E4:E9)</f>
-        <v>50</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10">
-        <f t="shared" ref="G10:M10" si="0">SUM(G4:G9)</f>
-        <v>6</v>
-      </c>
-      <c r="H10" s="10">
+      <c r="L10" s="46">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="M10" s="46">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="I10" s="10">
+      <c r="N10" s="46">
         <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="J10" s="10">
+        <v>109</v>
+      </c>
+      <c r="O10" s="46">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K10" s="10">
+      <c r="P10" s="46">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="10">
+        <v>21</v>
+      </c>
+      <c r="Q10" s="46">
         <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="M10" s="10">
+        <v>50</v>
+      </c>
+      <c r="R10" s="46">
         <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="S10" s="46">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="T10" s="46">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U10" s="46">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="V10" s="46">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="16" t="s">
+      <c r="F11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="J11" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="28" t="s">
+      <c r="K11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="M11" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="N11" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="O11" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="P11" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="Q11" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="26" t="s">
+      <c r="R11" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="18"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="T11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="U11" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="V11" s="41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12">
         <v>100</v>
-      </c>
-      <c r="D12">
-        <v>100</v>
-      </c>
-      <c r="E12">
-        <v>50</v>
-      </c>
-      <c r="G12">
-        <v>50</v>
-      </c>
-      <c r="H12">
-        <v>50</v>
       </c>
       <c r="I12">
         <v>100</v>
       </c>
       <c r="J12">
-        <v>100</v>
-      </c>
-      <c r="K12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>50</v>
       </c>
       <c r="M12">
+        <v>50</v>
+      </c>
+      <c r="N12">
+        <v>100</v>
+      </c>
+      <c r="O12">
+        <v>100</v>
+      </c>
+      <c r="P12">
+        <v>100</v>
+      </c>
+      <c r="Q12">
+        <v>50</v>
+      </c>
+      <c r="R12">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="e">
+        <f>ROUNDUP(B10/B12,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C13" t="e">
+        <f>ROUNDUP(C10/C12,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D13" t="e">
+        <f>ROUNDUP(D10/D12,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13">
+        <f>ROUNDUP(E10/E12,0)</f>
+        <v>2</v>
+      </c>
+      <c r="F13" t="e">
+        <f t="shared" ref="F13:V13" si="1">ROUNDUP(F10/F12,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="6">
         <v>4.6500000000000004</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6">
         <v>10.88</v>
       </c>
-      <c r="E13" s="19">
+      <c r="J14" s="50">
         <v>10</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19">
+      <c r="K14" s="6"/>
+      <c r="L14" s="6">
         <v>13.16</v>
       </c>
-      <c r="H13" s="19">
+      <c r="M14" s="6">
         <v>12.91</v>
       </c>
-      <c r="I13" s="19">
+      <c r="N14" s="6">
         <v>5.57</v>
       </c>
-      <c r="J13" s="19">
+      <c r="O14" s="6">
         <v>11.27</v>
       </c>
-      <c r="K13" s="19">
+      <c r="P14" s="6">
         <v>12.91</v>
       </c>
-      <c r="L13" s="19">
+      <c r="Q14" s="6">
         <v>14.3</v>
       </c>
-      <c r="M13" s="19">
+      <c r="R14" s="6">
         <v>13.72</v>
       </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="e">
-        <f>ROUNDUP(#REF!/B12,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D14" t="e">
-        <f>ROUNDUP(#REF!/D12,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E14" t="e">
-        <f>ROUNDUP(#REF!/E12,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G14" t="e">
-        <f>ROUNDUP(#REF!/G12,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H14" t="e">
-        <f>ROUNDUP(#REF!/H12,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I14" t="e">
-        <f>ROUNDUP(#REF!/I12,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J14" t="e">
-        <f>ROUNDUP(#REF!/J12,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K14" t="e">
-        <f>ROUNDUP(#REF!/K12,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L14" t="e">
-        <f>ROUNDUP(#REF!/L12,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M14" t="e">
-        <f>ROUNDUP(#REF!/M12,0)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="15" t="e">
-        <f>B14*B13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="e">
-        <f t="shared" ref="D15:M15" si="1">D14*D13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E15" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="H15" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I15" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="J15" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="K15" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="L15" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="M15" s="15" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="N15" s="21" t="e">
-        <f>SUM(B15:M15)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O15" s="22" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="48">
+        <f>E13*E14</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48">
+        <f>I13*I14</f>
+        <v>10.88</v>
+      </c>
+      <c r="J15" s="48">
+        <f>J13*J14</f>
+        <v>20</v>
+      </c>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48">
+        <f>L13*L14</f>
+        <v>13.16</v>
+      </c>
+      <c r="M15" s="48">
+        <f>M13*M14</f>
+        <v>12.91</v>
+      </c>
+      <c r="N15" s="48">
+        <f>N13*N14</f>
+        <v>11.14</v>
+      </c>
+      <c r="O15" s="48">
+        <f>O13*O14</f>
+        <v>11.27</v>
+      </c>
+      <c r="P15" s="48">
+        <f>P13*P14</f>
+        <v>12.91</v>
+      </c>
+      <c r="Q15" s="48">
+        <f>Q13*Q14</f>
+        <v>14.3</v>
+      </c>
+      <c r="R15" s="48">
+        <f>R13*R14</f>
+        <v>13.72</v>
+      </c>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="51">
+        <f>SUM(E15:R15)</f>
+        <v>129.59</v>
+      </c>
+      <c r="X15" s="52" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P16" s="13"/>
-      <c r="Q16" s="14"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="W17" s="13"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="13"/>
-      <c r="N20" t="s">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V16" s="4"/>
+      <c r="W16" s="5"/>
+    </row>
+    <row r="17" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="AC17" s="4"/>
+    </row>
+    <row r="18" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="I18" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+    </row>
+    <row r="19" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+    </row>
+    <row r="20" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="4"/>
+      <c r="S20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="K21" s="28"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G23" t="s">
-        <v>64</v>
-      </c>
-      <c r="N23" s="13"/>
-      <c r="P23" s="13"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G25" t="s">
-        <v>66</v>
-      </c>
+    <row r="21" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="P21" s="9"/>
+    </row>
+    <row r="22" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+    </row>
+    <row r="23" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="V23" s="4"/>
+    </row>
+    <row r="24" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+    </row>
+    <row r="25" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="N1:P1"/>
+  <mergeCells count="5">
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="I18:M25"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:M9 O4 O6">
+  <conditionalFormatting sqref="E9:G9 U4 U6 E4:F8 H8 J8:J9 I6:J7 I5:K5 I4:J4 N4:O4 L8:L9 N8 P8:Q8 M5:O7 Q4:R4 Q6:R6 Q5 Q7">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -1665,18 +1982,21 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="L11" r:id="rId1" display="https://www.mcmaster.com/91290A145" xr:uid="{EF0C7CB7-7F0C-4978-AD30-F63B825C607C}"/>
-    <hyperlink ref="J11" r:id="rId2" display="https://www.mcmaster.com/91290A144" xr:uid="{97946378-20E3-4BB5-A415-61DF7F90D13E}"/>
-    <hyperlink ref="E11" r:id="rId3" display="https://www.mcmaster.com/91290A572" xr:uid="{664D9FDE-70E3-4A0F-B351-35F0A3A2C3F5}"/>
-    <hyperlink ref="H11" r:id="rId4" display="https://www.mcmaster.com/91290A135" xr:uid="{9CA25500-E455-4F17-8A7E-0D4EF1250BFC}"/>
-    <hyperlink ref="D11" r:id="rId5" display="https://www.mcmaster.com/91290A117" xr:uid="{D77B4316-0FBE-4230-85B3-E918DE261303}"/>
-    <hyperlink ref="B11" r:id="rId6" display="https://www.mcmaster.com/90576A102" xr:uid="{1B492BCE-BBA3-4F43-A72C-90E5F22FA535}"/>
-    <hyperlink ref="I11" r:id="rId7" display="https://www.mcmaster.com/90576A103" xr:uid="{485778C1-91A9-4F26-B8D3-294C54C47869}"/>
-    <hyperlink ref="M11" r:id="rId8" display="https://www.mcmaster.com/91290A188" xr:uid="{A3E4A7F7-EEF8-4991-8FCD-F7DCFE2D5C14}"/>
-    <hyperlink ref="K11" r:id="rId9" display="https://www.mcmaster.com/91290A154" xr:uid="{BF65207D-35D8-4E2B-958E-E3273CAF7347}"/>
-    <hyperlink ref="G11" r:id="rId10" display="https://www.mcmaster.com/91290A130" xr:uid="{7A3866DF-7699-4781-B27F-F0645E8076DB}"/>
+    <hyperlink ref="Q11" r:id="rId1" display="https://www.mcmaster.com/91290A145" xr:uid="{EF0C7CB7-7F0C-4978-AD30-F63B825C607C}"/>
+    <hyperlink ref="O11" r:id="rId2" display="https://www.mcmaster.com/91290A144" xr:uid="{97946378-20E3-4BB5-A415-61DF7F90D13E}"/>
+    <hyperlink ref="J11" r:id="rId3" display="https://www.mcmaster.com/91290A572" xr:uid="{664D9FDE-70E3-4A0F-B351-35F0A3A2C3F5}"/>
+    <hyperlink ref="M11" r:id="rId4" display="https://www.mcmaster.com/91290A135" xr:uid="{9CA25500-E455-4F17-8A7E-0D4EF1250BFC}"/>
+    <hyperlink ref="I11" r:id="rId5" display="https://www.mcmaster.com/91290A117" xr:uid="{D77B4316-0FBE-4230-85B3-E918DE261303}"/>
+    <hyperlink ref="E11" r:id="rId6" display="https://www.mcmaster.com/90576A102" xr:uid="{1B492BCE-BBA3-4F43-A72C-90E5F22FA535}"/>
+    <hyperlink ref="N11" r:id="rId7" display="https://www.mcmaster.com/90576A103" xr:uid="{485778C1-91A9-4F26-B8D3-294C54C47869}"/>
+    <hyperlink ref="R11" r:id="rId8" display="https://www.mcmaster.com/91290A188" xr:uid="{A3E4A7F7-EEF8-4991-8FCD-F7DCFE2D5C14}"/>
+    <hyperlink ref="P11" r:id="rId9" display="https://www.mcmaster.com/91290A154" xr:uid="{BF65207D-35D8-4E2B-958E-E3273CAF7347}"/>
+    <hyperlink ref="L11" r:id="rId10" display="https://www.mcmaster.com/91290A130" xr:uid="{7A3866DF-7699-4781-B27F-F0645E8076DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
+  <ignoredErrors>
+    <ignoredError sqref="C10:R10" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished hardware count in BOM, still need to go track down links, identifier numbers and pricing
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EE05AA-E7BF-4BAB-94A4-940B09B1C9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD00987B-F087-4061-8F3A-A3CCDD95DFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46188" yWindow="-7152" windowWidth="46296" windowHeight="26136" activeTab="1" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
+    <workbookView xWindow="-39792" yWindow="-4116" windowWidth="34560" windowHeight="19188" activeTab="1" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
   <si>
     <t>Nut</t>
   </si>
@@ -211,9 +211,6 @@
     <t>8x22x7</t>
   </si>
   <si>
-    <t>0?</t>
-  </si>
-  <si>
     <t>M2.5</t>
   </si>
   <si>
@@ -223,9 +220,6 @@
     <t>30x37x4</t>
   </si>
   <si>
-    <t>WHAT SIZE SCREWS WERE USED TO ATTACH THE FINGERS TO THE CARRIER ADAPTERS? ADD THAT IN</t>
-  </si>
-  <si>
     <t>M2</t>
   </si>
   <si>
@@ -236,6 +230,21 @@
   </si>
   <si>
     <t>9XXXXXXXX</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>count total</t>
   </si>
 </sst>
 </file>
@@ -499,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -530,20 +539,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -582,12 +577,25 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1058,7 +1066,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1074,7 +1082,7 @@
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,100 +1096,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="46"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="49"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21">
+        <v>8</v>
+      </c>
+      <c r="D2" s="22">
+        <v>5</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="24">
+        <v>6</v>
+      </c>
+      <c r="H2" s="24">
+        <v>10</v>
+      </c>
+      <c r="I2" s="24">
+        <v>12</v>
+      </c>
+      <c r="J2" s="24">
+        <v>15</v>
+      </c>
+      <c r="K2" s="24">
+        <v>25</v>
+      </c>
+      <c r="L2" s="24">
+        <v>30</v>
+      </c>
+      <c r="M2" s="24">
+        <v>35</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="24">
+        <v>10</v>
+      </c>
+      <c r="P2" s="24">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="24">
+        <v>45</v>
+      </c>
+      <c r="R2" s="21">
+        <v>60</v>
+      </c>
+      <c r="S2" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="21"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="27">
-        <v>8</v>
-      </c>
-      <c r="D2" s="28">
-        <v>5</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="30">
-        <v>6</v>
-      </c>
-      <c r="H2" s="30">
-        <v>10</v>
-      </c>
-      <c r="I2" s="30">
-        <v>12</v>
-      </c>
-      <c r="J2" s="30">
-        <v>15</v>
-      </c>
-      <c r="K2" s="30">
-        <v>25</v>
-      </c>
-      <c r="L2" s="30">
-        <v>30</v>
-      </c>
-      <c r="M2" s="30">
-        <v>35</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="30">
-        <v>10</v>
-      </c>
-      <c r="P2" s="30">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="30">
-        <v>45</v>
-      </c>
-      <c r="R2" s="27">
+      <c r="T2" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="S2" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="T2" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="V2" s="27" t="s">
+      <c r="U2" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="21" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1189,89 +1197,89 @@
       <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="39"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
       <c r="M3" s="13"/>
-      <c r="N3" s="39">
+      <c r="N3" s="33">
         <v>17</v>
       </c>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40">
+      <c r="O3" s="34"/>
+      <c r="P3" s="34">
         <v>11</v>
       </c>
-      <c r="Q3" s="40"/>
+      <c r="Q3" s="34"/>
       <c r="R3" s="13">
         <v>6</v>
       </c>
-      <c r="S3" s="39"/>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
       <c r="V3" s="13"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27">
         <v>13</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="29">
         <v>4</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35">
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29">
         <v>8</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="29">
         <v>6</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="33">
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="27">
         <v>12</v>
       </c>
-      <c r="O4" s="35">
+      <c r="O4" s="29">
         <v>4</v>
       </c>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35">
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29">
         <v>6</v>
       </c>
-      <c r="R4" s="34">
+      <c r="R4" s="28">
         <v>6</v>
       </c>
-      <c r="S4" s="33">
+      <c r="S4" s="27">
         <v>2</v>
       </c>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35">
+      <c r="T4" s="29"/>
+      <c r="U4" s="29">
         <v>3</v>
       </c>
-      <c r="V4" s="34"/>
+      <c r="V4" s="28"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="16">
-        <v>29</v>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17">
+        <v>61</v>
       </c>
       <c r="F5" s="14">
         <v>8</v>
@@ -1282,17 +1290,17 @@
         <v>16</v>
       </c>
       <c r="J5" s="14">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K5" s="14">
         <v>3</v>
       </c>
       <c r="L5" s="14"/>
-      <c r="M5" s="24">
-        <v>6</v>
-      </c>
-      <c r="N5" s="16">
-        <v>44</v>
+      <c r="M5" s="18">
+        <v>21</v>
+      </c>
+      <c r="N5" s="17">
+        <v>24</v>
       </c>
       <c r="O5" s="14">
         <v>8</v>
@@ -1302,75 +1310,73 @@
         <v>24</v>
       </c>
       <c r="R5" s="14"/>
-      <c r="S5" s="23">
+      <c r="S5" s="17">
         <v>2</v>
       </c>
       <c r="T5" s="14"/>
       <c r="U5" s="14">
         <v>6</v>
       </c>
-      <c r="V5" s="24">
+      <c r="V5" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33">
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27">
         <v>13</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="29">
         <v>4</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35">
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29">
         <v>8</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="29">
         <v>6</v>
       </c>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="N6" s="33">
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="27">
         <v>12</v>
       </c>
-      <c r="O6" s="35">
+      <c r="O6" s="29">
         <v>4</v>
       </c>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35">
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29">
         <v>6</v>
       </c>
-      <c r="R6" s="34">
+      <c r="R6" s="28">
         <v>6</v>
       </c>
-      <c r="S6" s="33">
+      <c r="S6" s="27">
         <v>2</v>
       </c>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35">
+      <c r="T6" s="29"/>
+      <c r="U6" s="29">
         <v>3</v>
       </c>
-      <c r="V6" s="34">
+      <c r="V6" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17">
         <v>19</v>
       </c>
       <c r="F7" s="14">
@@ -1386,10 +1392,10 @@
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="24">
+      <c r="M7" s="18">
         <v>6</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="17">
         <v>12</v>
       </c>
       <c r="O7" s="14">
@@ -1400,62 +1406,62 @@
         <v>12</v>
       </c>
       <c r="R7" s="14"/>
-      <c r="S7" s="23">
+      <c r="S7" s="17">
         <v>1</v>
       </c>
       <c r="T7" s="14"/>
       <c r="U7" s="14">
         <v>3</v>
       </c>
-      <c r="V7" s="24">
+      <c r="V7" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="33">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="27">
         <v>8</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="27">
         <v>32</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="29">
         <v>8</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35">
+      <c r="G8" s="29"/>
+      <c r="H8" s="29">
         <v>16</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35">
+      <c r="I8" s="29"/>
+      <c r="J8" s="29">
         <v>12</v>
       </c>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35">
+      <c r="K8" s="29"/>
+      <c r="L8" s="29">
         <v>14</v>
       </c>
-      <c r="M8" s="35"/>
-      <c r="N8" s="33">
+      <c r="M8" s="29"/>
+      <c r="N8" s="27">
         <v>12</v>
       </c>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35">
+      <c r="O8" s="29"/>
+      <c r="P8" s="29">
         <v>10</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="29">
         <v>2</v>
       </c>
-      <c r="R8" s="35"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="35">
+      <c r="R8" s="29"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="29">
         <v>2</v>
       </c>
-      <c r="U8" s="35"/>
-      <c r="V8" s="34">
+      <c r="U8" s="29"/>
+      <c r="V8" s="28">
         <v>9</v>
       </c>
     </row>
@@ -1463,197 +1469,204 @@
       <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="30">
         <v>4</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="31">
+        <v>12</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30">
+        <v>12</v>
+      </c>
+      <c r="F9" s="32">
         <v>4</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36">
-        <v>12</v>
-      </c>
-      <c r="F9" s="38">
-        <v>4</v>
-      </c>
-      <c r="G9" s="38">
+      <c r="G9" s="32">
         <v>8</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="38">
+      <c r="J9" s="32">
         <v>12</v>
       </c>
       <c r="K9" s="14"/>
-      <c r="L9" s="38">
+      <c r="L9" s="32">
         <v>4</v>
       </c>
       <c r="M9" s="14"/>
-      <c r="N9" s="36"/>
+      <c r="N9" s="30"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
       <c r="R9" s="14"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
-      <c r="V9" s="37"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="31"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="40">
         <f>SUM(B3:B9)</f>
         <v>4</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="40">
         <f t="shared" ref="C10:V10" si="0">SUM(C3:C9)</f>
-        <v>4</v>
-      </c>
-      <c r="D10" s="46">
+        <v>12</v>
+      </c>
+      <c r="D10" s="40">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="40">
         <f t="shared" si="0"/>
-        <v>118</v>
-      </c>
-      <c r="F10" s="46">
+        <v>150</v>
+      </c>
+      <c r="F10" s="40">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="40">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="40">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I10" s="46">
+      <c r="I10" s="40">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="J10" s="46">
+      <c r="J10" s="40">
         <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="K10" s="46">
+        <v>62</v>
+      </c>
+      <c r="K10" s="40">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L10" s="46">
+      <c r="L10" s="40">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="M10" s="46">
+      <c r="M10" s="40">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="N10" s="46">
+        <v>27</v>
+      </c>
+      <c r="N10" s="40">
         <f t="shared" si="0"/>
-        <v>109</v>
-      </c>
-      <c r="O10" s="46">
+        <v>89</v>
+      </c>
+      <c r="O10" s="40">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P10" s="46">
+      <c r="P10" s="40">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Q10" s="46">
+      <c r="Q10" s="40">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="R10" s="46">
+      <c r="R10" s="40">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="S10" s="46">
+      <c r="S10" s="40">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="T10" s="46">
+      <c r="T10" s="40">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="U10" s="46">
+      <c r="U10" s="40">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="V10" s="46">
+      <c r="V10" s="40">
         <f t="shared" si="0"/>
         <v>14</v>
+      </c>
+      <c r="W10" s="51">
+        <f>SUM(B10:V10)</f>
+        <v>612</v>
+      </c>
+      <c r="X10" s="45" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="42" t="s">
+      <c r="B11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" s="43" t="s">
+      <c r="F11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="L11" s="44" t="s">
+      <c r="K11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="43" t="s">
+      <c r="M11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="42" t="s">
+      <c r="N11" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="42" t="s">
+      <c r="O11" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="45" t="s">
+      <c r="P11" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="42" t="s">
+      <c r="Q11" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="45" t="s">
+      <c r="R11" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="S11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="T11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="U11" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="V11" s="41" t="s">
-        <v>66</v>
+      <c r="S11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="T11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="U11" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="V11" s="35" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -1748,7 +1761,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O13">
         <f t="shared" si="1"/>
@@ -1799,7 +1812,7 @@
       <c r="I14" s="6">
         <v>10.88</v>
       </c>
-      <c r="J14" s="50">
+      <c r="J14" s="52">
         <v>10</v>
       </c>
       <c r="K14" s="6"/>
@@ -1830,65 +1843,65 @@
       <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="48">
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42">
         <f>E13*E14</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48">
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42">
         <f>I13*I14</f>
         <v>10.88</v>
       </c>
-      <c r="J15" s="48">
+      <c r="J15" s="42">
         <f>J13*J14</f>
         <v>20</v>
       </c>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48">
-        <f>L13*L14</f>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42">
+        <f t="shared" ref="L15:R15" si="2">L13*L14</f>
         <v>13.16</v>
       </c>
-      <c r="M15" s="48">
-        <f>M13*M14</f>
+      <c r="M15" s="42">
+        <f t="shared" si="2"/>
         <v>12.91</v>
       </c>
-      <c r="N15" s="48">
-        <f>N13*N14</f>
-        <v>11.14</v>
-      </c>
-      <c r="O15" s="48">
-        <f>O13*O14</f>
+      <c r="N15" s="42">
+        <f t="shared" si="2"/>
+        <v>5.57</v>
+      </c>
+      <c r="O15" s="42">
+        <f t="shared" si="2"/>
         <v>11.27</v>
       </c>
-      <c r="P15" s="48">
-        <f>P13*P14</f>
+      <c r="P15" s="42">
+        <f t="shared" si="2"/>
         <v>12.91</v>
       </c>
-      <c r="Q15" s="48">
-        <f>Q13*Q14</f>
+      <c r="Q15" s="42">
+        <f t="shared" si="2"/>
         <v>14.3</v>
       </c>
-      <c r="R15" s="48">
-        <f>R13*R14</f>
+      <c r="R15" s="42">
+        <f t="shared" si="2"/>
         <v>13.72</v>
       </c>
-      <c r="S15" s="49"/>
-      <c r="T15" s="49"/>
-      <c r="U15" s="49"/>
-      <c r="V15" s="49"/>
-      <c r="W15" s="51">
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="44">
         <f>SUM(E15:R15)</f>
-        <v>129.59</v>
-      </c>
-      <c r="X15" s="52" t="s">
+        <v>124.01999999999998</v>
+      </c>
+      <c r="X15" s="45" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1900,80 +1913,71 @@
       <c r="AC17" s="4"/>
     </row>
     <row r="18" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I18" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
     </row>
     <row r="19" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
     </row>
     <row r="20" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
       <c r="N20" s="4"/>
       <c r="S20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
       <c r="P21" s="9"/>
     </row>
     <row r="22" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
     </row>
     <row r="23" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
       <c r="V23" s="4"/>
     </row>
     <row r="24" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
     </row>
     <row r="25" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="E1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="S1:V1"/>
-    <mergeCell ref="I18:M25"/>
     <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:G9 U4 U6 E4:F8 H8 J8:J9 I6:J7 I5:K5 I4:J4 N4:O4 L8:L9 N8 P8:Q8 M5:O7 Q4:R4 Q6:R6 Q5 Q7">
+  <conditionalFormatting sqref="E9:G9 U4 U6 E4:F8 H8 J8:J9 I6:J7 I5:K5 I4:J4 N4:O4 L8:L9 N8 P8:Q8 M5:O5 Q4:R4 Q6:R6 Q5 Q7 M7:O7 N6:O6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Completed Hardware section of BOM with links and pricing included.  Minor change to dARM.3mf file to add fuzzy skin to TPU finger
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD00987B-F087-4061-8F3A-A3CCDD95DFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C819F517-562C-46D8-9666-FCB372BA17C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-39792" yWindow="-4116" windowWidth="34560" windowHeight="19188" activeTab="1" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>Nut</t>
   </si>
@@ -229,22 +229,40 @@
     <t>75x95x10</t>
   </si>
   <si>
-    <t>9XXXXXXXX</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>count total</t>
+  </si>
+  <si>
+    <t>6815-2RS</t>
+  </si>
+  <si>
+    <t>B0B93G1H9L</t>
+  </si>
+  <si>
+    <t>B0CXQ4QTGT</t>
+  </si>
+  <si>
+    <t>B07M7D9PRM</t>
+  </si>
+  <si>
+    <t>B082PS9PHD</t>
+  </si>
+  <si>
+    <t>B099DP2FN7</t>
+  </si>
+  <si>
+    <t>B01K1OUR84</t>
+  </si>
+  <si>
+    <t>91290A111</t>
+  </si>
+  <si>
+    <t>91290A115</t>
+  </si>
+  <si>
+    <t>91290A125</t>
+  </si>
+  <si>
+    <t>For many parts only a handful are actually needed but they are sold in very large pack sizes.  I recommend  attempting to source these somewhere else.</t>
   </si>
 </sst>
 </file>
@@ -279,7 +297,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -287,14 +305,14 @@
     </font>
     <font>
       <u/>
-      <sz val="8"/>
+      <sz val="7"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +343,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -508,7 +532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -516,14 +540,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -560,25 +582,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -591,11 +602,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1081,897 +1171,1012 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAFB602-290B-4982-B78B-7ABFBEFF08D7}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
+      <c r="A1" s="50"/>
+      <c r="B1" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="46"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="47" t="s">
+      <c r="O1" s="37"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="49"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="40"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="51"/>
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="19">
         <v>8</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="20">
         <v>5</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="22">
         <v>6</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="22">
         <v>10</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="22">
         <v>12</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="22">
         <v>15</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="22">
         <v>25</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="22">
         <v>30</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="22">
         <v>35</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="22">
         <v>10</v>
       </c>
-      <c r="P2" s="24">
+      <c r="P2" s="22">
         <v>16</v>
       </c>
-      <c r="Q2" s="24">
+      <c r="Q2" s="22">
         <v>45</v>
       </c>
-      <c r="R2" s="21">
+      <c r="R2" s="19">
         <v>60</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="S2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="33">
+      <c r="B3" s="31"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="31">
         <v>17</v>
       </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34">
+      <c r="O3" s="32"/>
+      <c r="P3" s="32">
         <v>11</v>
       </c>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="13">
+      <c r="Q3" s="32"/>
+      <c r="R3" s="11">
         <v>6</v>
       </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="13"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="11"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25">
         <v>13</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="27">
         <v>4</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29">
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27">
         <v>8</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="27">
         <v>6</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="27">
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="25">
         <v>12</v>
       </c>
-      <c r="O4" s="29">
+      <c r="O4" s="27">
         <v>4</v>
       </c>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29">
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27">
         <v>6</v>
       </c>
-      <c r="R4" s="28">
+      <c r="R4" s="26">
         <v>6</v>
       </c>
-      <c r="S4" s="27">
+      <c r="S4" s="25">
         <v>2</v>
       </c>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29">
+      <c r="T4" s="27"/>
+      <c r="U4" s="27">
         <v>3</v>
       </c>
-      <c r="V4" s="28"/>
+      <c r="V4" s="26"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15">
         <v>61</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>8</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14">
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12">
         <v>16</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="12">
         <v>20</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="12">
         <v>3</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="18">
+      <c r="L5" s="12"/>
+      <c r="M5" s="16">
         <v>21</v>
       </c>
-      <c r="N5" s="17">
+      <c r="N5" s="15">
         <v>24</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="12">
         <v>8</v>
       </c>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14">
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12">
         <v>24</v>
       </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="17">
+      <c r="R5" s="12"/>
+      <c r="S5" s="15">
         <v>2</v>
       </c>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14">
+      <c r="T5" s="12"/>
+      <c r="U5" s="12">
         <v>6</v>
       </c>
-      <c r="V5" s="18">
+      <c r="V5" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25">
         <v>13</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="27">
         <v>4</v>
       </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29">
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27">
         <v>8</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="27">
         <v>6</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="27">
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="25">
         <v>12</v>
       </c>
-      <c r="O6" s="29">
+      <c r="O6" s="27">
         <v>4</v>
       </c>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29">
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27">
         <v>6</v>
       </c>
-      <c r="R6" s="28">
+      <c r="R6" s="26">
         <v>6</v>
       </c>
-      <c r="S6" s="27">
+      <c r="S6" s="25">
         <v>2</v>
       </c>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29">
+      <c r="T6" s="27"/>
+      <c r="U6" s="27">
         <v>3</v>
       </c>
-      <c r="V6" s="28">
+      <c r="V6" s="26">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17">
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15">
         <v>19</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="12">
         <v>4</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14">
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12">
         <v>4</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="12">
         <v>6</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="18">
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="16">
         <v>6</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="15">
         <v>12</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="12">
         <v>4</v>
       </c>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14">
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12">
         <v>12</v>
       </c>
-      <c r="R7" s="14"/>
-      <c r="S7" s="17">
+      <c r="R7" s="12"/>
+      <c r="S7" s="15">
         <v>1</v>
       </c>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14">
+      <c r="T7" s="12"/>
+      <c r="U7" s="12">
         <v>3</v>
       </c>
-      <c r="V7" s="18">
+      <c r="V7" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="27">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="25">
         <v>8</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>32</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="27">
         <v>8</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29">
+      <c r="G8" s="27"/>
+      <c r="H8" s="27">
         <v>16</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29">
+      <c r="I8" s="27"/>
+      <c r="J8" s="27">
         <v>12</v>
       </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29">
+      <c r="K8" s="27"/>
+      <c r="L8" s="27">
         <v>14</v>
       </c>
-      <c r="M8" s="29"/>
-      <c r="N8" s="27">
+      <c r="M8" s="27"/>
+      <c r="N8" s="25">
         <v>12</v>
       </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29">
+      <c r="O8" s="27"/>
+      <c r="P8" s="27">
         <v>10</v>
       </c>
-      <c r="Q8" s="29">
+      <c r="Q8" s="27">
         <v>2</v>
       </c>
-      <c r="R8" s="29"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="29">
+      <c r="R8" s="27"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="27">
         <v>2</v>
       </c>
-      <c r="U8" s="29"/>
-      <c r="V8" s="28">
+      <c r="U8" s="27"/>
+      <c r="V8" s="26">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="28">
         <v>4</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="29">
         <v>12</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30">
+      <c r="D9" s="28"/>
+      <c r="E9" s="28">
         <v>12</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="30">
         <v>4</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="30">
         <v>8</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="32">
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="30">
         <v>12</v>
       </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="32">
+      <c r="K9" s="12"/>
+      <c r="L9" s="30">
         <v>4</v>
       </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="31"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="29"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="40">
-        <f>SUM(B3:B9)</f>
-        <v>4</v>
-      </c>
-      <c r="C10" s="40">
-        <f t="shared" ref="C10:V10" si="0">SUM(C3:C9)</f>
-        <v>12</v>
-      </c>
-      <c r="D10" s="40">
+      <c r="B10" s="64">
+        <f>SUM(B3:C9)</f>
+        <v>16</v>
+      </c>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65">
+        <f t="shared" ref="C10:V10" si="0">SUM(D3:D9)</f>
+        <v>8</v>
+      </c>
+      <c r="E10" s="66">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="F10" s="66">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="G10" s="66">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E10" s="40">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="F10" s="40">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="G10" s="40">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H10" s="40">
+      <c r="H10" s="66">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="66">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="J10" s="40">
+      <c r="J10" s="66">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="K10" s="40">
+      <c r="K10" s="66">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L10" s="40">
+      <c r="L10" s="66">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="M10" s="40">
+      <c r="M10" s="66">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="N10" s="40">
+      <c r="N10" s="72">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="O10" s="40">
+      <c r="O10" s="66">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P10" s="40">
+      <c r="P10" s="66">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Q10" s="40">
+      <c r="Q10" s="66">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="R10" s="40">
+      <c r="R10" s="66">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="S10" s="40">
+      <c r="S10" s="72">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="T10" s="40">
+      <c r="T10" s="66">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="U10" s="40">
+      <c r="U10" s="66">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="V10" s="40">
+      <c r="V10" s="67">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="W10" s="51">
+      <c r="W10" s="52">
         <f>SUM(B10:V10)</f>
         <v>612</v>
       </c>
-      <c r="X10" s="45" t="s">
+      <c r="X10" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="68"/>
+      <c r="D11" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="77" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="P11" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="R11" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="S11" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="T11" s="70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="L11" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="P11" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="R11" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="S11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="T11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="U11" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="V11" s="35" t="s">
-        <v>64</v>
+      <c r="U11" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="V11" s="71" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12">
+      <c r="B12" s="43">
+        <v>660</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="44">
+        <v>705</v>
+      </c>
+      <c r="E12" s="42">
         <v>100</v>
       </c>
-      <c r="I12">
+      <c r="F12" s="42">
+        <v>10</v>
+      </c>
+      <c r="G12" s="42">
         <v>100</v>
       </c>
-      <c r="J12">
+      <c r="H12" s="42">
+        <v>100</v>
+      </c>
+      <c r="I12" s="42">
+        <v>100</v>
+      </c>
+      <c r="J12" s="42">
         <v>50</v>
       </c>
-      <c r="L12">
+      <c r="K12" s="42">
+        <v>100</v>
+      </c>
+      <c r="L12" s="42">
         <v>50</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="42">
         <v>50</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="73">
         <v>100</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="42">
         <v>100</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="42">
         <v>100</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="42">
         <v>50</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="42">
         <v>25</v>
       </c>
+      <c r="S12" s="73">
+        <v>1</v>
+      </c>
+      <c r="T12" s="42">
+        <v>2</v>
+      </c>
+      <c r="U12" s="42">
+        <v>10</v>
+      </c>
+      <c r="V12" s="53">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="e">
+      <c r="B13" s="56">
         <f>ROUNDUP(B10/B12,0)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C13" t="e">
-        <f>ROUNDUP(C10/C12,0)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D13" t="e">
+        <v>1</v>
+      </c>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57">
         <f>ROUNDUP(D10/D12,0)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="41">
         <f>ROUNDUP(E10/E12,0)</f>
         <v>2</v>
       </c>
-      <c r="F13" t="e">
+      <c r="F13" s="41">
         <f t="shared" ref="F13:V13" si="1">ROUNDUP(F10/F12,0)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="G13" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="H13" s="41">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="41">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="41">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L13">
+      <c r="K13" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M13">
+      <c r="L13" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N13">
+      <c r="M13" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O13">
+      <c r="N13" s="74">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P13">
+      <c r="O13" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q13">
+      <c r="P13" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R13">
+      <c r="Q13" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="S13" t="e">
+      <c r="R13" s="41">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T13" t="e">
+        <v>1</v>
+      </c>
+      <c r="S13" s="74">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U13" t="e">
+        <v>7</v>
+      </c>
+      <c r="T13" s="41">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V13" t="e">
+        <v>1</v>
+      </c>
+      <c r="U13" s="41">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
+      </c>
+      <c r="V13" s="58">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="6">
+      <c r="B14" s="59">
+        <v>9.99</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="60">
+        <v>9.99</v>
+      </c>
+      <c r="E14" s="61">
         <v>4.6500000000000004</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6">
+      <c r="F14" s="61">
+        <v>6.79</v>
+      </c>
+      <c r="G14" s="61">
+        <v>11.32</v>
+      </c>
+      <c r="H14" s="61">
+        <v>12.92</v>
+      </c>
+      <c r="I14" s="61">
         <v>10.88</v>
       </c>
-      <c r="J14" s="52">
+      <c r="J14" s="62">
         <v>10</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6">
+      <c r="K14" s="61">
+        <v>17.37</v>
+      </c>
+      <c r="L14" s="61">
         <v>13.16</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="61">
         <v>12.91</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="75">
         <v>5.57</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="61">
         <v>11.27</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="61">
         <v>12.91</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q14" s="61">
         <v>14.3</v>
       </c>
-      <c r="R14" s="6">
+      <c r="R14" s="61">
         <v>13.72</v>
       </c>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
+      <c r="S14" s="75">
+        <v>15.79</v>
+      </c>
+      <c r="T14" s="61">
+        <v>8.49</v>
+      </c>
+      <c r="U14" s="61">
+        <v>9.99</v>
+      </c>
+      <c r="V14" s="63">
+        <v>7.99</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42">
+      <c r="B15" s="45">
+        <f>B14*B13</f>
+        <v>9.99</v>
+      </c>
+      <c r="C15" s="45"/>
+      <c r="D15" s="46">
+        <f>D14*D13</f>
+        <v>9.99</v>
+      </c>
+      <c r="E15" s="47">
         <f>E13*E14</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42">
-        <f>I13*I14</f>
+      <c r="F15" s="47">
+        <f t="shared" ref="F15:V15" si="2">F13*F14</f>
+        <v>27.16</v>
+      </c>
+      <c r="G15" s="47">
+        <f t="shared" si="2"/>
+        <v>11.32</v>
+      </c>
+      <c r="H15" s="47">
+        <f t="shared" si="2"/>
+        <v>12.92</v>
+      </c>
+      <c r="I15" s="47">
+        <f t="shared" si="2"/>
         <v>10.88</v>
       </c>
-      <c r="J15" s="42">
-        <f>J13*J14</f>
+      <c r="J15" s="47">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42">
-        <f t="shared" ref="L15:R15" si="2">L13*L14</f>
+      <c r="K15" s="47">
+        <f t="shared" si="2"/>
+        <v>17.37</v>
+      </c>
+      <c r="L15" s="47">
+        <f t="shared" si="2"/>
         <v>13.16</v>
       </c>
-      <c r="M15" s="42">
+      <c r="M15" s="47">
         <f t="shared" si="2"/>
         <v>12.91</v>
       </c>
-      <c r="N15" s="42">
+      <c r="N15" s="76">
         <f t="shared" si="2"/>
         <v>5.57</v>
       </c>
-      <c r="O15" s="42">
+      <c r="O15" s="47">
         <f t="shared" si="2"/>
         <v>11.27</v>
       </c>
-      <c r="P15" s="42">
+      <c r="P15" s="47">
         <f t="shared" si="2"/>
         <v>12.91</v>
       </c>
-      <c r="Q15" s="42">
+      <c r="Q15" s="47">
         <f t="shared" si="2"/>
         <v>14.3</v>
       </c>
-      <c r="R15" s="42">
+      <c r="R15" s="47">
         <f t="shared" si="2"/>
         <v>13.72</v>
       </c>
-      <c r="S15" s="43"/>
-      <c r="T15" s="43"/>
-      <c r="U15" s="43"/>
-      <c r="V15" s="43"/>
-      <c r="W15" s="44">
-        <f>SUM(E15:R15)</f>
-        <v>124.01999999999998</v>
-      </c>
-      <c r="X15" s="45" t="s">
+      <c r="S15" s="76">
+        <f t="shared" si="2"/>
+        <v>110.53</v>
+      </c>
+      <c r="T15" s="47">
+        <f t="shared" si="2"/>
+        <v>8.49</v>
+      </c>
+      <c r="U15" s="47">
+        <f t="shared" si="2"/>
+        <v>19.98</v>
+      </c>
+      <c r="V15" s="48">
+        <f t="shared" si="2"/>
+        <v>15.98</v>
+      </c>
+      <c r="W15" s="34">
+        <f>SUM(B15:R15)</f>
+        <v>212.76999999999998</v>
+      </c>
+      <c r="X15" s="35" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="V16" s="4"/>
-      <c r="W16" s="5"/>
-    </row>
-    <row r="17" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="AC17" s="4"/>
-    </row>
-    <row r="18" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-    </row>
-    <row r="19" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-    </row>
-    <row r="20" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="4"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="4"/>
+    </row>
+    <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="AC17" s="3"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="55"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="55"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="55"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="3"/>
       <c r="S20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="P21" s="9"/>
-    </row>
-    <row r="22" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-    </row>
-    <row r="23" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="V23" s="4"/>
-    </row>
-    <row r="24" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I24" s="50"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
-    </row>
-    <row r="25" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="50"/>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="P21" s="7"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="V23" s="3"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="12">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A17:F20"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="E1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="S1:V1"/>
@@ -1990,17 +2195,27 @@
     <hyperlink ref="O11" r:id="rId2" display="https://www.mcmaster.com/91290A144" xr:uid="{97946378-20E3-4BB5-A415-61DF7F90D13E}"/>
     <hyperlink ref="J11" r:id="rId3" display="https://www.mcmaster.com/91290A572" xr:uid="{664D9FDE-70E3-4A0F-B351-35F0A3A2C3F5}"/>
     <hyperlink ref="M11" r:id="rId4" display="https://www.mcmaster.com/91290A135" xr:uid="{9CA25500-E455-4F17-8A7E-0D4EF1250BFC}"/>
-    <hyperlink ref="I11" r:id="rId5" display="https://www.mcmaster.com/91290A117" xr:uid="{D77B4316-0FBE-4230-85B3-E918DE261303}"/>
-    <hyperlink ref="E11" r:id="rId6" display="https://www.mcmaster.com/90576A102" xr:uid="{1B492BCE-BBA3-4F43-A72C-90E5F22FA535}"/>
-    <hyperlink ref="N11" r:id="rId7" display="https://www.mcmaster.com/90576A103" xr:uid="{485778C1-91A9-4F26-B8D3-294C54C47869}"/>
-    <hyperlink ref="R11" r:id="rId8" display="https://www.mcmaster.com/91290A188" xr:uid="{A3E4A7F7-EEF8-4991-8FCD-F7DCFE2D5C14}"/>
-    <hyperlink ref="P11" r:id="rId9" display="https://www.mcmaster.com/91290A154" xr:uid="{BF65207D-35D8-4E2B-958E-E3273CAF7347}"/>
-    <hyperlink ref="L11" r:id="rId10" display="https://www.mcmaster.com/91290A130" xr:uid="{7A3866DF-7699-4781-B27F-F0645E8076DB}"/>
+    <hyperlink ref="E11" r:id="rId5" display="https://www.mcmaster.com/90576A102" xr:uid="{1B492BCE-BBA3-4F43-A72C-90E5F22FA535}"/>
+    <hyperlink ref="N11" r:id="rId6" display="https://www.mcmaster.com/90576A103" xr:uid="{485778C1-91A9-4F26-B8D3-294C54C47869}"/>
+    <hyperlink ref="R11" r:id="rId7" display="https://www.mcmaster.com/91290A188" xr:uid="{A3E4A7F7-EEF8-4991-8FCD-F7DCFE2D5C14}"/>
+    <hyperlink ref="P11" r:id="rId8" display="https://www.mcmaster.com/91290A154" xr:uid="{BF65207D-35D8-4E2B-958E-E3273CAF7347}"/>
+    <hyperlink ref="S11" r:id="rId9" xr:uid="{F3AB31F2-9BD7-46E3-8A99-22C43A088240}"/>
+    <hyperlink ref="B11:C11" r:id="rId10" display="B0B93G1H9L" xr:uid="{50E51E63-8C87-45F8-8325-EC0E503A272F}"/>
+    <hyperlink ref="D11" r:id="rId11" xr:uid="{66BC059A-B148-4CC0-B8CA-C0587255B50F}"/>
+    <hyperlink ref="F11" r:id="rId12" xr:uid="{E7F37B86-3D5D-4B4F-97FB-1013D3F05906}"/>
+    <hyperlink ref="T11" r:id="rId13" xr:uid="{079C2E76-0A71-4E1A-8E17-E14E23C0A551}"/>
+    <hyperlink ref="V11" r:id="rId14" xr:uid="{7E6A892D-7AA8-4CAB-91DD-88F943EFDE7E}"/>
+    <hyperlink ref="U11" r:id="rId15" xr:uid="{7C230941-0BCD-4050-B193-D66AE312B306}"/>
+    <hyperlink ref="I11" r:id="rId16" display="https://www.mcmaster.com/91290A117" xr:uid="{D77B4316-0FBE-4230-85B3-E918DE261303}"/>
+    <hyperlink ref="G11" r:id="rId17" xr:uid="{06F82045-714F-4836-9F06-941804A17887}"/>
+    <hyperlink ref="H11" r:id="rId18" xr:uid="{3A5131C6-94AE-49D2-B0F3-B50050AA3F9A}"/>
+    <hyperlink ref="L11" r:id="rId19" display="https://www.mcmaster.com/91290A130" xr:uid="{7A3866DF-7699-4781-B27F-F0645E8076DB}"/>
+    <hyperlink ref="K11" r:id="rId20" xr:uid="{2C38CA73-687E-4AD4-8546-52A176EB9FA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
   <ignoredErrors>
-    <ignoredError sqref="C10:R10" formulaRange="1"/>
+    <ignoredError sqref="D10:R10" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished BOM, for now, total price $2,117.53 not including filament
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C819F517-562C-46D8-9666-FCB372BA17C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1A6277-FDB6-46EF-B70C-607EAFD96DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39792" yWindow="-4116" windowWidth="34560" windowHeight="19188" activeTab="1" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
+    <workbookView xWindow="-39516" yWindow="-3840" windowWidth="34560" windowHeight="19188" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
   <si>
     <t>Nut</t>
   </si>
@@ -121,72 +121,15 @@
     <t>Gripper</t>
   </si>
   <si>
-    <t>Wires Standard</t>
-  </si>
-  <si>
-    <t>Wires Forearm</t>
-  </si>
-  <si>
-    <t>Wires Gripper</t>
-  </si>
-  <si>
-    <t>Bolts</t>
-  </si>
-  <si>
-    <t>Nuts</t>
-  </si>
-  <si>
-    <t>Encoder Magnets</t>
-  </si>
-  <si>
     <t>ODrives S1</t>
   </si>
   <si>
-    <t>Power Supply</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/dp/B0C298NSS4</t>
-  </si>
-  <si>
     <t>Power Monitor</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B0CZ36J9BY</t>
-  </si>
-  <si>
-    <t>Slider = MGN7C, 100mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> https://www.aliexpress.us/item/3256804722090559.html</t>
-  </si>
-  <si>
-    <t>Motor = GM5208-24</t>
-  </si>
-  <si>
-    <t>https://upgraderc.be/en/products/iflight-ipower-gm5208-12-24-gimbal-motor?variant=46529548419396</t>
-  </si>
-  <si>
-    <t>Motor = GB36-2</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.us/item/1281133501.html</t>
-  </si>
-  <si>
-    <t>Motor = EaglePower 8308 90KV</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.us/item/3256807861814061.html</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Total Price</t>
   </si>
   <si>
@@ -196,15 +139,9 @@
     <t>Raspberry Pi 4 Model B</t>
   </si>
   <si>
-    <t>https://www.adafruit.com/product/4564?src=raspberrypi</t>
-  </si>
-  <si>
     <t>Bearings</t>
   </si>
   <si>
-    <t>Standoffs</t>
-  </si>
-  <si>
     <t>Standoff</t>
   </si>
   <si>
@@ -214,9 +151,6 @@
     <t>M2.5</t>
   </si>
   <si>
-    <t>Belts - 300mm GT2</t>
-  </si>
-  <si>
     <t>30x37x4</t>
   </si>
   <si>
@@ -263,6 +197,72 @@
   </si>
   <si>
     <t>For many parts only a handful are actually needed but they are sold in very large pack sizes.  I recommend  attempting to source these somewhere else.</t>
+  </si>
+  <si>
+    <t>Encoder Magnets (5 Pack)</t>
+  </si>
+  <si>
+    <t>Wires Standard (14 AWG)</t>
+  </si>
+  <si>
+    <t>Wires Forearm/Gripper (18 AWG)</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Motors</t>
+  </si>
+  <si>
+    <t>EaglePower 8308 90KV</t>
+  </si>
+  <si>
+    <t>GB36-2</t>
+  </si>
+  <si>
+    <t>GM5208-24</t>
+  </si>
+  <si>
+    <t>Controll</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Sacrificial JST GH 4 Pin Wires</t>
+  </si>
+  <si>
+    <t>Twisted Pair (100 Ft)</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>MGN7C Rail 100mm and Carrier Block</t>
+  </si>
+  <si>
+    <t>MGN7C Carrier Block</t>
+  </si>
+  <si>
+    <t>GT2 Belts (300mm)</t>
+  </si>
+  <si>
+    <t>Bolts, Nuts, and Pulleys</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>see hardware sheet</t>
+  </si>
+  <si>
+    <t>total price</t>
+  </si>
+  <si>
+    <t>48V 25A 1200W Switching Power Supply</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -312,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +349,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -532,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -590,28 +596,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -621,28 +609,13 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -650,9 +623,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -660,9 +630,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -684,6 +651,74 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1021,149 +1056,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CD22FD-255E-455F-872D-D755421F4957}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="90"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="83">
+        <v>85.99</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="83">
+        <f>C3*B3</f>
+        <v>85.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="81" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="84"/>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="84">
+        <v>13.88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="84">
+        <v>21.88</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="84">
+        <f>C5*B5</f>
+        <v>21.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="86">
+        <v>13.88</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1</v>
+      </c>
+      <c r="D6" s="86">
+        <f>C6*B6</f>
+        <v>13.88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="93"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="83">
+        <v>42.99</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="83">
+        <f>C8*B8</f>
+        <v>42.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="81" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="84">
+        <v>61.35</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="84">
+        <f>C9*B9</f>
+        <v>122.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="81" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="86">
+        <v>53</v>
+      </c>
+      <c r="C10" s="10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="86">
+        <f>C10*B10</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="90"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="81" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" s="83">
+        <v>149</v>
+      </c>
+      <c r="C12" s="8">
+        <v>8</v>
+      </c>
+      <c r="D12" s="83">
+        <f>C12*B12</f>
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="84">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2</v>
+      </c>
+      <c r="D13" s="84">
+        <f>C13*B13</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15">
+      <c r="B14" s="86">
         <v>75</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
+      <c r="C14" s="10">
+        <v>1</v>
+      </c>
+      <c r="D14" s="86">
+        <f>C14*B14</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="92"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="93"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="83">
+        <v>9.99</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="83">
+        <f>C16*B16</f>
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="81" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="86">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="C17" s="10">
+        <v>1</v>
+      </c>
+      <c r="D17" s="86">
+        <f>C17*B17</f>
+        <v>17.440000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="90"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="83">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="83">
+        <f>C19*B19</f>
+        <v>8.4499999999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="81" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="84">
+        <v>4.57</v>
+      </c>
+      <c r="C20" s="9">
+        <v>1</v>
+      </c>
+      <c r="D20" s="84">
+        <f>C20*B20</f>
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="84">
+        <v>12.99</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="84">
+        <f t="shared" ref="D21" si="0">C21*B21</f>
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="82" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="86">
+        <f>Hardware!W15</f>
+        <v>212.76999999999998</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="79"/>
+      <c r="D23" s="34">
+        <f>SUM(D19:D22,D16:D17,D12:D14,D8:D10,D3:D6)</f>
+        <v>2117.5300000000002</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="79"/>
+      <c r="D24" s="79"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A18:D18"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="48V 25A 1200W DC Switching Power Supply" xr:uid="{C5468CE6-9D80-4F99-9755-3B3EC496B147}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{C48D4976-132F-410B-978C-02AAFE267A50}"/>
+    <hyperlink ref="A12" r:id="rId3" xr:uid="{20B0A697-5465-4668-9700-959AE063FEFE}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{5616C467-0CAC-4DB0-AB8B-9CF650AEE797}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{69894006-C14A-4461-A1C6-A5CCE40780FF}"/>
+    <hyperlink ref="A14" r:id="rId6" xr:uid="{9C47EDF3-11B8-49D1-9C3A-FBA96D7FD82E}"/>
+    <hyperlink ref="A13" r:id="rId7" xr:uid="{BD7E260E-D4A7-4D81-93B3-F421B8E00846}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{595B5008-BB6D-4AE7-BD6E-1C5E4738F0EA}"/>
+    <hyperlink ref="A9" r:id="rId9" xr:uid="{E61C0645-2B50-42C9-A91D-3F39CE5BF703}"/>
+    <hyperlink ref="A8" r:id="rId10" xr:uid="{1856345F-7308-4DAC-8B48-5EAA3057FB25}"/>
+    <hyperlink ref="A16" r:id="rId11" xr:uid="{0D91CE6A-66D2-4EE3-8AD6-97349C317CB1}"/>
+    <hyperlink ref="A17" r:id="rId12" display="Twisted Pair" xr:uid="{5B5135CB-772C-4BA9-B079-326FC4985EC7}"/>
+    <hyperlink ref="A19" r:id="rId13" display="Slider = MGN7C, 100mm" xr:uid="{352AA45C-A4FB-450E-9CEE-C1EB506FD5FF}"/>
+    <hyperlink ref="A20" r:id="rId14" xr:uid="{92FFB630-A737-4037-9E58-4FA6C83EAC94}"/>
+    <hyperlink ref="A21" r:id="rId15" xr:uid="{3F62A2E2-11F2-4AB9-9F02-0746567A5A81}"/>
+    <hyperlink ref="A22" location="Hardware!A1" display="Bolts, Nuts, and Pulleys" xr:uid="{63683D99-0A3B-4A5B-B17A-9D7D8C81AB20}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -1171,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAFB602-290B-4982-B78B-7ABFBEFF08D7}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,41 +1437,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="50"/>
-      <c r="B1" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="40"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="78"/>
       <c r="D1" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="37"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
       <c r="R1" s="6"/>
-      <c r="S1" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="40"/>
+      <c r="S1" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="78"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
+      <c r="A2" s="68"/>
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1243,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="G2" s="22">
         <v>6</v>
@@ -1282,16 +1524,16 @@
         <v>60</v>
       </c>
       <c r="S2" s="18" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="T2" s="23" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="U2" s="23" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -1610,224 +1852,224 @@
       <c r="A10" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="64">
+      <c r="B10" s="72">
         <f>SUM(B3:C9)</f>
         <v>16</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="65">
-        <f t="shared" ref="C10:V10" si="0">SUM(D3:D9)</f>
+      <c r="C10" s="72"/>
+      <c r="D10" s="53">
+        <f t="shared" ref="D10:V10" si="0">SUM(D3:D9)</f>
         <v>8</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="54">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="F10" s="66">
+      <c r="F10" s="54">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="G10" s="66">
+      <c r="G10" s="54">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="54">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I10" s="66">
+      <c r="I10" s="54">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="J10" s="66">
+      <c r="J10" s="54">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="K10" s="66">
+      <c r="K10" s="54">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L10" s="66">
+      <c r="L10" s="54">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="M10" s="66">
+      <c r="M10" s="54">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="N10" s="72">
+      <c r="N10" s="59">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="O10" s="66">
+      <c r="O10" s="54">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P10" s="66">
+      <c r="P10" s="54">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Q10" s="66">
+      <c r="Q10" s="54">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="R10" s="66">
+      <c r="R10" s="54">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="S10" s="72">
+      <c r="S10" s="59">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="T10" s="66">
+      <c r="T10" s="54">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="U10" s="66">
+      <c r="U10" s="54">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="V10" s="67">
+      <c r="V10" s="55">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="W10" s="52">
+      <c r="W10" s="44">
         <f>SUM(B10:V10)</f>
         <v>612</v>
       </c>
       <c r="X10" s="35" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="70" t="s">
+      <c r="B11" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="70"/>
+      <c r="D11" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="70" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="70" t="s">
+      <c r="F11" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="70" t="s">
+      <c r="J11" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="L11" s="78" t="s">
+      <c r="K11" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="70" t="s">
+      <c r="M11" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="77" t="s">
+      <c r="N11" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="70" t="s">
+      <c r="O11" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="70" t="s">
+      <c r="P11" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="70" t="s">
+      <c r="Q11" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="70" t="s">
+      <c r="R11" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="S11" s="77" t="s">
-        <v>65</v>
-      </c>
-      <c r="T11" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="U11" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="V11" s="71" t="s">
-        <v>70</v>
+      <c r="S11" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="T11" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="U11" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="V11" s="58" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="43">
+      <c r="B12" s="71">
         <v>660</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44">
+      <c r="C12" s="71"/>
+      <c r="D12" s="39">
         <v>705</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="38">
         <v>100</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="38">
         <v>10</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="38">
         <v>100</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="38">
         <v>100</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="38">
         <v>100</v>
       </c>
-      <c r="J12" s="42">
+      <c r="J12" s="38">
         <v>50</v>
       </c>
-      <c r="K12" s="42">
+      <c r="K12" s="38">
         <v>100</v>
       </c>
-      <c r="L12" s="42">
+      <c r="L12" s="38">
         <v>50</v>
       </c>
-      <c r="M12" s="42">
+      <c r="M12" s="38">
         <v>50</v>
       </c>
-      <c r="N12" s="73">
+      <c r="N12" s="60">
         <v>100</v>
       </c>
-      <c r="O12" s="42">
+      <c r="O12" s="38">
         <v>100</v>
       </c>
-      <c r="P12" s="42">
+      <c r="P12" s="38">
         <v>100</v>
       </c>
-      <c r="Q12" s="42">
+      <c r="Q12" s="38">
         <v>50</v>
       </c>
-      <c r="R12" s="42">
+      <c r="R12" s="38">
         <v>25</v>
       </c>
-      <c r="S12" s="73">
-        <v>1</v>
-      </c>
-      <c r="T12" s="42">
+      <c r="S12" s="60">
+        <v>1</v>
+      </c>
+      <c r="T12" s="38">
         <v>2</v>
       </c>
-      <c r="U12" s="42">
+      <c r="U12" s="38">
         <v>10</v>
       </c>
-      <c r="V12" s="53">
+      <c r="V12" s="45">
         <v>10</v>
       </c>
     </row>
@@ -1835,84 +2077,84 @@
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="56">
+      <c r="B13" s="73">
         <f>ROUNDUP(B10/B12,0)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57">
+      <c r="C13" s="73"/>
+      <c r="D13" s="47">
         <f>ROUNDUP(D10/D12,0)</f>
         <v>1</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="37">
         <f>ROUNDUP(E10/E12,0)</f>
         <v>2</v>
       </c>
-      <c r="F13" s="41">
+      <c r="F13" s="37">
         <f t="shared" ref="F13:V13" si="1">ROUNDUP(F10/F12,0)</f>
         <v>4</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H13" s="41">
+      <c r="H13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I13" s="41">
+      <c r="I13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J13" s="41">
+      <c r="J13" s="37">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K13" s="41">
+      <c r="K13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L13" s="41">
+      <c r="L13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M13" s="41">
+      <c r="M13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N13" s="74">
+      <c r="N13" s="61">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O13" s="41">
+      <c r="O13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P13" s="41">
+      <c r="P13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q13" s="41">
+      <c r="Q13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R13" s="41">
+      <c r="R13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="S13" s="74">
+      <c r="S13" s="61">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="T13" s="41">
+      <c r="T13" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="U13" s="41">
+      <c r="U13" s="37">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="V13" s="58">
+      <c r="V13" s="48">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1921,150 +2163,150 @@
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="59">
+      <c r="B14" s="74">
         <v>9.99</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60">
+      <c r="C14" s="74"/>
+      <c r="D14" s="49">
         <v>9.99</v>
       </c>
-      <c r="E14" s="61">
+      <c r="E14" s="50">
         <v>4.6500000000000004</v>
       </c>
-      <c r="F14" s="61">
+      <c r="F14" s="50">
         <v>6.79</v>
       </c>
-      <c r="G14" s="61">
+      <c r="G14" s="50">
         <v>11.32</v>
       </c>
-      <c r="H14" s="61">
+      <c r="H14" s="50">
         <v>12.92</v>
       </c>
-      <c r="I14" s="61">
+      <c r="I14" s="50">
         <v>10.88</v>
       </c>
-      <c r="J14" s="62">
+      <c r="J14" s="51">
         <v>10</v>
       </c>
-      <c r="K14" s="61">
+      <c r="K14" s="50">
         <v>17.37</v>
       </c>
-      <c r="L14" s="61">
+      <c r="L14" s="50">
         <v>13.16</v>
       </c>
-      <c r="M14" s="61">
+      <c r="M14" s="50">
         <v>12.91</v>
       </c>
-      <c r="N14" s="75">
+      <c r="N14" s="62">
         <v>5.57</v>
       </c>
-      <c r="O14" s="61">
+      <c r="O14" s="50">
         <v>11.27</v>
       </c>
-      <c r="P14" s="61">
+      <c r="P14" s="50">
         <v>12.91</v>
       </c>
-      <c r="Q14" s="61">
+      <c r="Q14" s="50">
         <v>14.3</v>
       </c>
-      <c r="R14" s="61">
+      <c r="R14" s="50">
         <v>13.72</v>
       </c>
-      <c r="S14" s="75">
+      <c r="S14" s="62">
         <v>15.79</v>
       </c>
-      <c r="T14" s="61">
+      <c r="T14" s="50">
         <v>8.49</v>
       </c>
-      <c r="U14" s="61">
+      <c r="U14" s="50">
         <v>9.99</v>
       </c>
-      <c r="V14" s="63">
+      <c r="V14" s="52">
         <v>7.99</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="45">
+      <c r="B15" s="66">
         <f>B14*B13</f>
         <v>9.99</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="46">
+      <c r="C15" s="66"/>
+      <c r="D15" s="40">
         <f>D14*D13</f>
         <v>9.99</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="41">
         <f>E13*E14</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F15" s="41">
         <f t="shared" ref="F15:V15" si="2">F13*F14</f>
         <v>27.16</v>
       </c>
-      <c r="G15" s="47">
+      <c r="G15" s="41">
         <f t="shared" si="2"/>
         <v>11.32</v>
       </c>
-      <c r="H15" s="47">
+      <c r="H15" s="41">
         <f t="shared" si="2"/>
         <v>12.92</v>
       </c>
-      <c r="I15" s="47">
+      <c r="I15" s="41">
         <f t="shared" si="2"/>
         <v>10.88</v>
       </c>
-      <c r="J15" s="47">
+      <c r="J15" s="41">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K15" s="47">
+      <c r="K15" s="41">
         <f t="shared" si="2"/>
         <v>17.37</v>
       </c>
-      <c r="L15" s="47">
+      <c r="L15" s="41">
         <f t="shared" si="2"/>
         <v>13.16</v>
       </c>
-      <c r="M15" s="47">
+      <c r="M15" s="41">
         <f t="shared" si="2"/>
         <v>12.91</v>
       </c>
-      <c r="N15" s="76">
+      <c r="N15" s="63">
         <f t="shared" si="2"/>
         <v>5.57</v>
       </c>
-      <c r="O15" s="47">
+      <c r="O15" s="41">
         <f t="shared" si="2"/>
         <v>11.27</v>
       </c>
-      <c r="P15" s="47">
+      <c r="P15" s="41">
         <f t="shared" si="2"/>
         <v>12.91</v>
       </c>
-      <c r="Q15" s="47">
+      <c r="Q15" s="41">
         <f t="shared" si="2"/>
         <v>14.3</v>
       </c>
-      <c r="R15" s="47">
+      <c r="R15" s="41">
         <f t="shared" si="2"/>
         <v>13.72</v>
       </c>
-      <c r="S15" s="76">
+      <c r="S15" s="63">
         <f t="shared" si="2"/>
         <v>110.53</v>
       </c>
-      <c r="T15" s="47">
+      <c r="T15" s="41">
         <f t="shared" si="2"/>
         <v>8.49</v>
       </c>
-      <c r="U15" s="47">
+      <c r="U15" s="41">
         <f t="shared" si="2"/>
         <v>19.98</v>
       </c>
-      <c r="V15" s="48">
+      <c r="V15" s="42">
         <f t="shared" si="2"/>
         <v>15.98</v>
       </c>
@@ -2081,47 +2323,47 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
+      <c r="A17" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
       <c r="AC17" s="3"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
+      <c r="A18" s="69"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
       <c r="M18" s="36"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="36"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="55"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="36"/>
@@ -2168,7 +2410,11 @@
       <c r="M25" s="36"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="12">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A17:F20"/>
@@ -2178,9 +2424,6 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="E1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:G9 U4 U6 E4:F8 H8 J8:J9 I6:J7 I5:K5 I4:J4 N4:O4 L8:L9 N8 P8:Q8 M5:O5 Q4:R4 Q6:R6 Q5 Q7 M7:O7 N6:O6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Added wire t connectors and weights to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1A6277-FDB6-46EF-B70C-607EAFD96DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BA1DC1-D499-4F3A-A59C-205CB7DABDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39516" yWindow="-3840" windowWidth="34560" windowHeight="19188" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
+    <workbookView xWindow="-39240" yWindow="-3564" windowWidth="34560" windowHeight="19188" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>Nut</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Wire T Connectors</t>
+  </si>
+  <si>
+    <t>Weights</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -653,45 +659,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
@@ -721,6 +688,49 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1056,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CD22FD-255E-455F-872D-D755421F4957}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,341 +1081,376 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="74" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="90"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="77"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="83">
+      <c r="B3" s="70">
         <v>85.99</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
       </c>
-      <c r="D3" s="83">
+      <c r="D3" s="70">
         <f>C3*B3</f>
         <v>85.99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="84"/>
+      <c r="B4" s="71">
+        <v>13.88</v>
+      </c>
       <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="D4" s="84">
+      <c r="D4" s="71">
+        <f>C4*B4</f>
         <v>13.88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="84">
+      <c r="B5" s="71">
         <v>21.88</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
       </c>
-      <c r="D5" s="84">
+      <c r="D5" s="71">
         <f>C5*B5</f>
         <v>21.88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="86">
+      <c r="B6" s="71">
         <v>13.88</v>
       </c>
-      <c r="C6" s="10">
-        <v>1</v>
-      </c>
-      <c r="D6" s="86">
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="71">
         <f>C6*B6</f>
         <v>13.88</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="94">
+        <v>14.99</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="73">
+        <f>C7*B7</f>
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="93"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="81" t="s">
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="80"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="83">
+      <c r="B9" s="70">
         <v>42.99</v>
       </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="83">
-        <f>C8*B8</f>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="70">
+        <f>C9*B9</f>
         <v>42.99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="81" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="84">
+      <c r="B10" s="71">
         <v>61.35</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C10" s="9">
         <v>2</v>
       </c>
-      <c r="D9" s="84">
-        <f>C9*B9</f>
+      <c r="D10" s="71">
+        <f>C10*B10</f>
         <v>122.7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="81" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="86">
+      <c r="B11" s="73">
         <v>53</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C11" s="10">
         <v>5</v>
       </c>
-      <c r="D10" s="86">
-        <f>C10*B10</f>
+      <c r="D11" s="73">
+        <f>C11*B11</f>
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="88" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="89"/>
-      <c r="C11" s="89"/>
-      <c r="D11" s="90"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="81" t="s">
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="77"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="83">
+      <c r="B13" s="70">
         <v>149</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C13" s="8">
         <v>8</v>
       </c>
-      <c r="D12" s="83">
-        <f>C12*B12</f>
+      <c r="D13" s="70">
+        <f>C13*B13</f>
         <v>1192</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="81" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="84">
+      <c r="B14" s="71">
         <v>9</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C14" s="9">
         <v>2</v>
       </c>
-      <c r="D13" s="84">
-        <f>C13*B13</f>
+      <c r="D14" s="71">
+        <f>C14*B14</f>
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="81" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="86">
+      <c r="B15" s="73">
         <v>75</v>
       </c>
-      <c r="C14" s="10">
-        <v>1</v>
-      </c>
-      <c r="D14" s="86">
-        <f>C14*B14</f>
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" s="73">
+        <f>C15*B15</f>
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="91" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="92"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="93"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="81" t="s">
+      <c r="B16" s="79"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="80"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="83">
+      <c r="B17" s="70">
         <v>9.99</v>
       </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-      <c r="D16" s="83">
-        <f>C16*B16</f>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="70">
+        <f>C17*B17</f>
         <v>9.99</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="81" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="86">
+      <c r="B18" s="73">
         <v>17.440000000000001</v>
       </c>
-      <c r="C17" s="10">
-        <v>1</v>
-      </c>
-      <c r="D17" s="86">
-        <f>C17*B17</f>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="73">
+        <f>C18*B18</f>
         <v>17.440000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="88" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="89"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="90"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="81" t="s">
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="77"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="97" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="95">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="C20" s="96">
+        <v>3</v>
+      </c>
+      <c r="D20" s="70">
+        <f>C20*B20</f>
+        <v>56.97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="83">
+      <c r="B21" s="71">
         <v>8.4499999999999993</v>
       </c>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="83">
-        <f>C19*B19</f>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="71">
+        <f>C21*B21</f>
         <v>8.4499999999999993</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="81" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="84">
+      <c r="B22" s="71">
         <v>4.57</v>
       </c>
-      <c r="C20" s="9">
-        <v>1</v>
-      </c>
-      <c r="D20" s="84">
-        <f>C20*B20</f>
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
+      <c r="D22" s="71">
+        <f>C22*B22</f>
         <v>4.57</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="81" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="84">
+      <c r="B23" s="71">
         <v>12.99</v>
       </c>
-      <c r="C21" s="9">
-        <v>1</v>
-      </c>
-      <c r="D21" s="84">
-        <f t="shared" ref="D21" si="0">C21*B21</f>
+      <c r="C23" s="9">
+        <v>1</v>
+      </c>
+      <c r="D23" s="71">
+        <f t="shared" ref="D23" si="0">C23*B23</f>
         <v>12.99</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="82" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="85" t="s">
+      <c r="B24" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="85" t="s">
+      <c r="C24" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="86">
+      <c r="D24" s="73">
         <f>Hardware!W15</f>
         <v>212.76999999999998</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E24" s="38" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="79"/>
-      <c r="D23" s="34">
-        <f>SUM(D19:D22,D16:D17,D12:D14,D8:D10,D3:D6)</f>
-        <v>2117.5300000000002</v>
-      </c>
-      <c r="E23" s="35" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="66"/>
+      <c r="D25" s="34">
+        <f>SUM(D20:D24,D17:D18,D13:D15,D9:D11,D3:D7)</f>
+        <v>2189.4900000000002</v>
+      </c>
+      <c r="E25" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="79"/>
-      <c r="D24" s="79"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="66"/>
+      <c r="D26" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A19:D19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="48V 25A 1200W DC Switching Power Supply" xr:uid="{C5468CE6-9D80-4F99-9755-3B3EC496B147}"/>
     <hyperlink ref="A4" r:id="rId2" xr:uid="{C48D4976-132F-410B-978C-02AAFE267A50}"/>
-    <hyperlink ref="A12" r:id="rId3" xr:uid="{20B0A697-5465-4668-9700-959AE063FEFE}"/>
+    <hyperlink ref="A13" r:id="rId3" xr:uid="{20B0A697-5465-4668-9700-959AE063FEFE}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{5616C467-0CAC-4DB0-AB8B-9CF650AEE797}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{69894006-C14A-4461-A1C6-A5CCE40780FF}"/>
-    <hyperlink ref="A14" r:id="rId6" xr:uid="{9C47EDF3-11B8-49D1-9C3A-FBA96D7FD82E}"/>
-    <hyperlink ref="A13" r:id="rId7" xr:uid="{BD7E260E-D4A7-4D81-93B3-F421B8E00846}"/>
-    <hyperlink ref="A10" r:id="rId8" xr:uid="{595B5008-BB6D-4AE7-BD6E-1C5E4738F0EA}"/>
-    <hyperlink ref="A9" r:id="rId9" xr:uid="{E61C0645-2B50-42C9-A91D-3F39CE5BF703}"/>
-    <hyperlink ref="A8" r:id="rId10" xr:uid="{1856345F-7308-4DAC-8B48-5EAA3057FB25}"/>
-    <hyperlink ref="A16" r:id="rId11" xr:uid="{0D91CE6A-66D2-4EE3-8AD6-97349C317CB1}"/>
-    <hyperlink ref="A17" r:id="rId12" display="Twisted Pair" xr:uid="{5B5135CB-772C-4BA9-B079-326FC4985EC7}"/>
-    <hyperlink ref="A19" r:id="rId13" display="Slider = MGN7C, 100mm" xr:uid="{352AA45C-A4FB-450E-9CEE-C1EB506FD5FF}"/>
-    <hyperlink ref="A20" r:id="rId14" xr:uid="{92FFB630-A737-4037-9E58-4FA6C83EAC94}"/>
-    <hyperlink ref="A21" r:id="rId15" xr:uid="{3F62A2E2-11F2-4AB9-9F02-0746567A5A81}"/>
-    <hyperlink ref="A22" location="Hardware!A1" display="Bolts, Nuts, and Pulleys" xr:uid="{63683D99-0A3B-4A5B-B17A-9D7D8C81AB20}"/>
+    <hyperlink ref="A15" r:id="rId6" xr:uid="{9C47EDF3-11B8-49D1-9C3A-FBA96D7FD82E}"/>
+    <hyperlink ref="A14" r:id="rId7" xr:uid="{BD7E260E-D4A7-4D81-93B3-F421B8E00846}"/>
+    <hyperlink ref="A11" r:id="rId8" xr:uid="{595B5008-BB6D-4AE7-BD6E-1C5E4738F0EA}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{E61C0645-2B50-42C9-A91D-3F39CE5BF703}"/>
+    <hyperlink ref="A9" r:id="rId10" xr:uid="{1856345F-7308-4DAC-8B48-5EAA3057FB25}"/>
+    <hyperlink ref="A17" r:id="rId11" xr:uid="{0D91CE6A-66D2-4EE3-8AD6-97349C317CB1}"/>
+    <hyperlink ref="A18" r:id="rId12" display="Twisted Pair" xr:uid="{5B5135CB-772C-4BA9-B079-326FC4985EC7}"/>
+    <hyperlink ref="A21" r:id="rId13" display="Slider = MGN7C, 100mm" xr:uid="{352AA45C-A4FB-450E-9CEE-C1EB506FD5FF}"/>
+    <hyperlink ref="A22" r:id="rId14" xr:uid="{92FFB630-A737-4037-9E58-4FA6C83EAC94}"/>
+    <hyperlink ref="A23" r:id="rId15" xr:uid="{3F62A2E2-11F2-4AB9-9F02-0746567A5A81}"/>
+    <hyperlink ref="A24" location="Hardware!A1" display="Bolts, Nuts, and Pulleys" xr:uid="{63683D99-0A3B-4A5B-B17A-9D7D8C81AB20}"/>
+    <hyperlink ref="A7" r:id="rId16" xr:uid="{F5EE5609-133A-47EC-8B0D-0F30E5401954}"/>
+    <hyperlink ref="A20" r:id="rId17" xr:uid="{9AEFC194-D90C-48DF-8BDE-F55DE7023DEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -1437,41 +1482,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="67"/>
-      <c r="B1" s="76" t="s">
+      <c r="A1" s="86"/>
+      <c r="B1" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="78"/>
+      <c r="C1" s="84"/>
       <c r="D1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="75" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75" t="s">
+      <c r="E1" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="75"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
       <c r="R1" s="6"/>
-      <c r="S1" s="76" t="s">
+      <c r="S1" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="78"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="84"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="68"/>
+      <c r="A2" s="87"/>
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1852,11 +1897,11 @@
       <c r="A10" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="72">
+      <c r="B10" s="91">
         <f>SUM(B3:C9)</f>
         <v>16</v>
       </c>
-      <c r="C10" s="72"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="53">
         <f t="shared" ref="D10:V10" si="0">SUM(D3:D9)</f>
         <v>8</v>
@@ -1945,10 +1990,10 @@
       <c r="A11" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="70"/>
+      <c r="C11" s="89"/>
       <c r="D11" s="56" t="s">
         <v>45</v>
       </c>
@@ -2011,10 +2056,10 @@
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="71">
+      <c r="B12" s="90">
         <v>660</v>
       </c>
-      <c r="C12" s="71"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="39">
         <v>705</v>
       </c>
@@ -2077,11 +2122,11 @@
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="73">
+      <c r="B13" s="92">
         <f>ROUNDUP(B10/B12,0)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="73"/>
+      <c r="C13" s="92"/>
       <c r="D13" s="47">
         <f>ROUNDUP(D10/D12,0)</f>
         <v>1</v>
@@ -2163,10 +2208,10 @@
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="74">
+      <c r="B14" s="93">
         <v>9.99</v>
       </c>
-      <c r="C14" s="74"/>
+      <c r="C14" s="93"/>
       <c r="D14" s="49">
         <v>9.99</v>
       </c>
@@ -2229,11 +2274,11 @@
       <c r="A15" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="66">
+      <c r="B15" s="85">
         <f>B14*B13</f>
         <v>9.99</v>
       </c>
-      <c r="C15" s="66"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="40">
         <f>D14*D13</f>
         <v>9.99</v>
@@ -2323,47 +2368,47 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
       <c r="AC17" s="3"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="69"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
       <c r="M18" s="36"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="69"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="36"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="69"/>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="36"/>
@@ -2412,17 +2457,17 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="12">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="A17:F20"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:G9 U4 U6 E4:F8 H8 J8:J9 I6:J7 I5:K5 I4:J4 N4:O4 L8:L9 N8 P8:Q8 M5:O5 Q4:R4 Q6:R6 Q5 Q7 M7:O7 N6:O6">

</xml_diff>

<commit_message>
Added rubber grommets and power switch to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BA1DC1-D499-4F3A-A59C-205CB7DABDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EF1F76-238C-4AC9-ADCF-4EBEA7950E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39240" yWindow="-3564" windowWidth="34560" windowHeight="19188" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
+    <workbookView xWindow="-38964" yWindow="-3288" windowWidth="34560" windowHeight="19188" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
   <si>
     <t>Nut</t>
   </si>
@@ -269,6 +269,12 @@
   </si>
   <si>
     <t>Weights</t>
+  </si>
+  <si>
+    <t>Power Switch</t>
+  </si>
+  <si>
+    <t>Rubber Grommets</t>
   </si>
 </sst>
 </file>
@@ -670,67 +676,67 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1066,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CD22FD-255E-455F-872D-D755421F4957}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,12 +1101,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
@@ -1134,323 +1140,354 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B5" s="71">
-        <v>21.88</v>
+        <v>10.99</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
       </c>
       <c r="D5" s="71">
         <f>C5*B5</f>
-        <v>21.88</v>
+        <v>10.99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B6" s="71">
-        <v>13.88</v>
+        <v>4.29</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
       </c>
       <c r="D6" s="71">
         <f>C6*B6</f>
-        <v>13.88</v>
+        <v>4.29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="94">
-        <v>14.99</v>
-      </c>
-      <c r="C7" s="10">
-        <v>1</v>
-      </c>
-      <c r="D7" s="73">
+        <v>55</v>
+      </c>
+      <c r="B7" s="71">
+        <v>21.88</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="71">
         <f>C7*B7</f>
-        <v>14.99</v>
+        <v>21.88</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
+      <c r="A8" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="71">
+        <v>13.88</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="71">
+        <f>C8*B8</f>
+        <v>13.88</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="68" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="70">
-        <v>42.99</v>
-      </c>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="70">
+        <v>76</v>
+      </c>
+      <c r="B9" s="75">
+        <v>14.99</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
+      </c>
+      <c r="D9" s="73">
         <f>C9*B9</f>
-        <v>42.99</v>
+        <v>14.99</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="71">
-        <v>61.35</v>
-      </c>
-      <c r="C10" s="9">
-        <v>2</v>
-      </c>
-      <c r="D10" s="71">
-        <f>C10*B10</f>
-        <v>122.7</v>
-      </c>
+      <c r="A10" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="83"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="84"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="68" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="73">
-        <v>53</v>
-      </c>
-      <c r="C11" s="10">
-        <v>5</v>
-      </c>
-      <c r="D11" s="73">
+        <v>61</v>
+      </c>
+      <c r="B11" s="70">
+        <v>42.99</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="70">
         <f>C11*B11</f>
-        <v>265</v>
+        <v>42.99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="75" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="77"/>
+      <c r="A12" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="71">
+        <v>61.35</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2</v>
+      </c>
+      <c r="D12" s="71">
+        <f>C12*B12</f>
+        <v>122.7</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="70">
-        <v>149</v>
-      </c>
-      <c r="C13" s="8">
-        <v>8</v>
-      </c>
-      <c r="D13" s="70">
+        <v>59</v>
+      </c>
+      <c r="B13" s="73">
+        <v>53</v>
+      </c>
+      <c r="C13" s="10">
+        <v>5</v>
+      </c>
+      <c r="D13" s="73">
         <f>C13*B13</f>
-        <v>1192</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="71">
-        <v>9</v>
-      </c>
-      <c r="C14" s="9">
-        <v>2</v>
-      </c>
-      <c r="D14" s="71">
-        <f>C14*B14</f>
-        <v>18</v>
-      </c>
+      <c r="A14" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="73">
-        <v>75</v>
-      </c>
-      <c r="C15" s="10">
-        <v>1</v>
-      </c>
-      <c r="D15" s="73">
+        <v>28</v>
+      </c>
+      <c r="B15" s="70">
+        <v>149</v>
+      </c>
+      <c r="C15" s="8">
+        <v>8</v>
+      </c>
+      <c r="D15" s="70">
         <f>C15*B15</f>
-        <v>75</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="78" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="80"/>
+      <c r="A16" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="71">
+        <v>9</v>
+      </c>
+      <c r="C16" s="9">
+        <v>2</v>
+      </c>
+      <c r="D16" s="71">
+        <f>C16*B16</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="73">
+        <v>75</v>
+      </c>
+      <c r="C17" s="10">
+        <v>1</v>
+      </c>
+      <c r="D17" s="73">
+        <f>C17*B17</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="83"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="84"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="70">
+      <c r="B19" s="70">
         <v>9.99</v>
       </c>
-      <c r="C17" s="8">
-        <v>1</v>
-      </c>
-      <c r="D17" s="70">
-        <f>C17*B17</f>
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="70">
+        <f>C19*B19</f>
         <v>9.99</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="68" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="73">
+      <c r="B20" s="73">
         <v>17.440000000000001</v>
       </c>
-      <c r="C18" s="10">
-        <v>1</v>
-      </c>
-      <c r="D18" s="73">
-        <f>C18*B18</f>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="73">
+        <f>C20*B20</f>
         <v>17.440000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="75" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="77"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="97" t="s">
+      <c r="B21" s="80"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="81"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="95">
+      <c r="B22" s="76">
         <v>18.989999999999998</v>
       </c>
-      <c r="C20" s="96">
+      <c r="C22" s="77">
         <v>3</v>
       </c>
-      <c r="D20" s="70">
-        <f>C20*B20</f>
+      <c r="D22" s="70">
+        <f>C22*B22</f>
         <v>56.97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="68" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="71">
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="C21" s="9">
-        <v>1</v>
-      </c>
-      <c r="D21" s="71">
-        <f>C21*B21</f>
-        <v>8.4499999999999993</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="71">
-        <v>4.57</v>
-      </c>
-      <c r="C22" s="9">
-        <v>1</v>
-      </c>
-      <c r="D22" s="71">
-        <f>C22*B22</f>
-        <v>4.57</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="71">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="C23" s="9">
+        <v>1</v>
+      </c>
+      <c r="D23" s="71">
+        <f>C23*B23</f>
+        <v>8.4499999999999993</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="71">
+        <v>4.57</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="71">
+        <f>C24*B24</f>
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="71">
+      <c r="B25" s="71">
         <v>12.99</v>
       </c>
-      <c r="C23" s="9">
-        <v>1</v>
-      </c>
-      <c r="D23" s="71">
-        <f t="shared" ref="D23" si="0">C23*B23</f>
+      <c r="C25" s="9">
+        <v>1</v>
+      </c>
+      <c r="D25" s="71">
+        <f t="shared" ref="D25" si="0">C25*B25</f>
         <v>12.99</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="69" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="72" t="s">
+      <c r="B26" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="72" t="s">
+      <c r="C26" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="73">
+      <c r="D26" s="73">
         <f>Hardware!W15</f>
         <v>212.76999999999998</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E26" s="38" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="66"/>
-      <c r="D25" s="34">
-        <f>SUM(D20:D24,D17:D18,D13:D15,D9:D11,D3:D7)</f>
-        <v>2189.4900000000002</v>
-      </c>
-      <c r="E25" s="35" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="66"/>
+      <c r="D27" s="34">
+        <f>SUM(D22:D26,D19:D20,D15:D17,D11:D13,D3:D9)</f>
+        <v>2204.77</v>
+      </c>
+      <c r="E27" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="66"/>
-      <c r="D26" s="66"/>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="66"/>
+      <c r="D28" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="48V 25A 1200W DC Switching Power Supply" xr:uid="{C5468CE6-9D80-4F99-9755-3B3EC496B147}"/>
     <hyperlink ref="A4" r:id="rId2" xr:uid="{C48D4976-132F-410B-978C-02AAFE267A50}"/>
-    <hyperlink ref="A13" r:id="rId3" xr:uid="{20B0A697-5465-4668-9700-959AE063FEFE}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{5616C467-0CAC-4DB0-AB8B-9CF650AEE797}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{69894006-C14A-4461-A1C6-A5CCE40780FF}"/>
-    <hyperlink ref="A15" r:id="rId6" xr:uid="{9C47EDF3-11B8-49D1-9C3A-FBA96D7FD82E}"/>
-    <hyperlink ref="A14" r:id="rId7" xr:uid="{BD7E260E-D4A7-4D81-93B3-F421B8E00846}"/>
-    <hyperlink ref="A11" r:id="rId8" xr:uid="{595B5008-BB6D-4AE7-BD6E-1C5E4738F0EA}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{E61C0645-2B50-42C9-A91D-3F39CE5BF703}"/>
-    <hyperlink ref="A9" r:id="rId10" xr:uid="{1856345F-7308-4DAC-8B48-5EAA3057FB25}"/>
-    <hyperlink ref="A17" r:id="rId11" xr:uid="{0D91CE6A-66D2-4EE3-8AD6-97349C317CB1}"/>
-    <hyperlink ref="A18" r:id="rId12" display="Twisted Pair" xr:uid="{5B5135CB-772C-4BA9-B079-326FC4985EC7}"/>
-    <hyperlink ref="A21" r:id="rId13" display="Slider = MGN7C, 100mm" xr:uid="{352AA45C-A4FB-450E-9CEE-C1EB506FD5FF}"/>
-    <hyperlink ref="A22" r:id="rId14" xr:uid="{92FFB630-A737-4037-9E58-4FA6C83EAC94}"/>
-    <hyperlink ref="A23" r:id="rId15" xr:uid="{3F62A2E2-11F2-4AB9-9F02-0746567A5A81}"/>
-    <hyperlink ref="A24" location="Hardware!A1" display="Bolts, Nuts, and Pulleys" xr:uid="{63683D99-0A3B-4A5B-B17A-9D7D8C81AB20}"/>
-    <hyperlink ref="A7" r:id="rId16" xr:uid="{F5EE5609-133A-47EC-8B0D-0F30E5401954}"/>
-    <hyperlink ref="A20" r:id="rId17" xr:uid="{9AEFC194-D90C-48DF-8BDE-F55DE7023DEE}"/>
+    <hyperlink ref="A15" r:id="rId3" xr:uid="{20B0A697-5465-4668-9700-959AE063FEFE}"/>
+    <hyperlink ref="A7" r:id="rId4" xr:uid="{5616C467-0CAC-4DB0-AB8B-9CF650AEE797}"/>
+    <hyperlink ref="A8" r:id="rId5" xr:uid="{69894006-C14A-4461-A1C6-A5CCE40780FF}"/>
+    <hyperlink ref="A17" r:id="rId6" xr:uid="{9C47EDF3-11B8-49D1-9C3A-FBA96D7FD82E}"/>
+    <hyperlink ref="A16" r:id="rId7" xr:uid="{BD7E260E-D4A7-4D81-93B3-F421B8E00846}"/>
+    <hyperlink ref="A13" r:id="rId8" xr:uid="{595B5008-BB6D-4AE7-BD6E-1C5E4738F0EA}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{E61C0645-2B50-42C9-A91D-3F39CE5BF703}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{1856345F-7308-4DAC-8B48-5EAA3057FB25}"/>
+    <hyperlink ref="A19" r:id="rId11" xr:uid="{0D91CE6A-66D2-4EE3-8AD6-97349C317CB1}"/>
+    <hyperlink ref="A20" r:id="rId12" display="Twisted Pair" xr:uid="{5B5135CB-772C-4BA9-B079-326FC4985EC7}"/>
+    <hyperlink ref="A23" r:id="rId13" display="Slider = MGN7C, 100mm" xr:uid="{352AA45C-A4FB-450E-9CEE-C1EB506FD5FF}"/>
+    <hyperlink ref="A24" r:id="rId14" xr:uid="{92FFB630-A737-4037-9E58-4FA6C83EAC94}"/>
+    <hyperlink ref="A25" r:id="rId15" xr:uid="{3F62A2E2-11F2-4AB9-9F02-0746567A5A81}"/>
+    <hyperlink ref="A26" location="Hardware!A1" display="Bolts, Nuts, and Pulleys" xr:uid="{63683D99-0A3B-4A5B-B17A-9D7D8C81AB20}"/>
+    <hyperlink ref="A9" r:id="rId16" xr:uid="{F5EE5609-133A-47EC-8B0D-0F30E5401954}"/>
+    <hyperlink ref="A22" r:id="rId17" xr:uid="{9AEFC194-D90C-48DF-8BDE-F55DE7023DEE}"/>
+    <hyperlink ref="A5" r:id="rId18" xr:uid="{F18F67CE-F323-4551-B427-8B044FAC8855}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -1482,41 +1519,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="82" t="s">
+      <c r="A1" s="96"/>
+      <c r="B1" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="84"/>
+      <c r="C1" s="94"/>
       <c r="D1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81" t="s">
+      <c r="E1" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="81"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
       <c r="R1" s="6"/>
-      <c r="S1" s="82" t="s">
+      <c r="S1" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="84"/>
+      <c r="T1" s="93"/>
+      <c r="U1" s="93"/>
+      <c r="V1" s="94"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="87"/>
+      <c r="A2" s="97"/>
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1897,11 +1934,11 @@
       <c r="A10" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="91">
+      <c r="B10" s="88">
         <f>SUM(B3:C9)</f>
         <v>16</v>
       </c>
-      <c r="C10" s="91"/>
+      <c r="C10" s="88"/>
       <c r="D10" s="53">
         <f t="shared" ref="D10:V10" si="0">SUM(D3:D9)</f>
         <v>8</v>
@@ -1990,10 +2027,10 @@
       <c r="A11" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="89"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="56" t="s">
         <v>45</v>
       </c>
@@ -2056,10 +2093,10 @@
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="90">
+      <c r="B12" s="87">
         <v>660</v>
       </c>
-      <c r="C12" s="90"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="39">
         <v>705</v>
       </c>
@@ -2122,11 +2159,11 @@
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="92">
+      <c r="B13" s="89">
         <f>ROUNDUP(B10/B12,0)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="92"/>
+      <c r="C13" s="89"/>
       <c r="D13" s="47">
         <f>ROUNDUP(D10/D12,0)</f>
         <v>1</v>
@@ -2208,10 +2245,10 @@
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="93">
+      <c r="B14" s="90">
         <v>9.99</v>
       </c>
-      <c r="C14" s="93"/>
+      <c r="C14" s="90"/>
       <c r="D14" s="49">
         <v>9.99</v>
       </c>
@@ -2274,11 +2311,11 @@
       <c r="A15" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="85">
+      <c r="B15" s="95">
         <f>B14*B13</f>
         <v>9.99</v>
       </c>
-      <c r="C15" s="85"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="40">
         <f>D14*D13</f>
         <v>9.99</v>
@@ -2368,47 +2405,47 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="88"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
       <c r="AC17" s="3"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
-      <c r="B18" s="88"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
       <c r="M18" s="36"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="36"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
+      <c r="A20" s="85"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="36"/>
@@ -2457,18 +2494,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="12">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:M1"/>
     <mergeCell ref="A17:F20"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:G9 U4 U6 E4:F8 H8 J8:J9 I6:J7 I5:K5 I4:J4 N4:O4 L8:L9 N8 P8:Q8 M5:O5 Q4:R4 Q6:R6 Q5 Q7 M7:O7 N6:O6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Added RS485 CAN Hat to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EF1F76-238C-4AC9-ADCF-4EBEA7950E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81D7F8E-516F-4274-979A-8AD029CF1E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38964" yWindow="-3288" windowWidth="34560" windowHeight="19188" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
@@ -226,9 +226,6 @@
     <t>Controll</t>
   </si>
   <si>
-    <t>Communication</t>
-  </si>
-  <si>
     <t>Sacrificial JST GH 4 Pin Wires</t>
   </si>
   <si>
@@ -275,6 +272,9 @@
   </si>
   <si>
     <t>Rubber Grommets</t>
+  </si>
+  <si>
+    <t>RS485 CAN HAT</t>
   </si>
 </sst>
 </file>
@@ -698,6 +698,27 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -714,27 +735,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1075,7 +1075,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1094,7 @@
         <v>32</v>
       </c>
       <c r="C1" s="74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="74" t="s">
         <v>31</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="70">
         <v>85.99</v>
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="70">
-        <f>C3*B3</f>
+        <f t="shared" ref="D3:D9" si="0">C3*B3</f>
         <v>85.99</v>
       </c>
     </row>
@@ -1134,13 +1134,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="71">
-        <f>C4*B4</f>
+        <f t="shared" si="0"/>
         <v>13.88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="71">
         <v>10.99</v>
@@ -1149,13 +1149,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="71">
-        <f>C5*B5</f>
+        <f t="shared" si="0"/>
         <v>10.99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="71">
         <v>4.29</v>
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="71">
-        <f>C6*B6</f>
+        <f t="shared" si="0"/>
         <v>4.29</v>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="71">
-        <f>C7*B7</f>
+        <f t="shared" si="0"/>
         <v>21.88</v>
       </c>
     </row>
@@ -1194,13 +1194,13 @@
         <v>1</v>
       </c>
       <c r="D8" s="71">
-        <f>C8*B8</f>
+        <f t="shared" si="0"/>
         <v>13.88</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="68" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="75">
         <v>14.99</v>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="73">
-        <f>C9*B9</f>
+        <f t="shared" si="0"/>
         <v>14.99</v>
       </c>
     </row>
@@ -1308,43 +1308,50 @@
       <c r="A17" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="73">
+      <c r="B17" s="71">
         <v>75</v>
       </c>
-      <c r="C17" s="10">
-        <v>1</v>
-      </c>
-      <c r="D17" s="73">
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="71">
         <f>C17*B17</f>
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="84"/>
+      <c r="A18" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="71">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="71">
+        <f>C18*B18</f>
+        <v>16.309999999999999</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="70">
+        <v>63</v>
+      </c>
+      <c r="B19" s="71">
         <v>9.99</v>
       </c>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="70">
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+      <c r="D19" s="71">
         <f>C19*B19</f>
         <v>9.99</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="73">
         <v>17.440000000000001</v>
@@ -1359,7 +1366,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="80"/>
       <c r="C21" s="80"/>
@@ -1367,7 +1374,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="76">
         <v>18.989999999999998</v>
@@ -1382,7 +1389,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="71">
         <v>8.4499999999999993</v>
@@ -1397,7 +1404,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" s="71">
         <v>4.57</v>
@@ -1412,7 +1419,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="71">
         <v>12.99</v>
@@ -1421,26 +1428,26 @@
         <v>1</v>
       </c>
       <c r="D25" s="71">
-        <f t="shared" ref="D25" si="0">C25*B25</f>
+        <f t="shared" ref="D25" si="1">C25*B25</f>
         <v>12.99</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="72" t="s">
-        <v>71</v>
-      </c>
       <c r="C26" s="72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" s="73">
         <f>Hardware!W15</f>
         <v>212.76999999999998</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1450,7 +1457,7 @@
         <v>2204.77</v>
       </c>
       <c r="E27" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1458,11 +1465,10 @@
       <c r="D28" s="66"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A18:D18"/>
     <mergeCell ref="A21:D21"/>
   </mergeCells>
   <hyperlinks>
@@ -1485,9 +1491,10 @@
     <hyperlink ref="A9" r:id="rId16" xr:uid="{F5EE5609-133A-47EC-8B0D-0F30E5401954}"/>
     <hyperlink ref="A22" r:id="rId17" xr:uid="{9AEFC194-D90C-48DF-8BDE-F55DE7023DEE}"/>
     <hyperlink ref="A5" r:id="rId18" xr:uid="{F18F67CE-F323-4551-B427-8B044FAC8855}"/>
+    <hyperlink ref="A18" r:id="rId19" xr:uid="{69B9BDE9-053E-49E8-B136-8E72FF6296E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -1519,41 +1526,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="96"/>
-      <c r="B1" s="92" t="s">
+      <c r="A1" s="90"/>
+      <c r="B1" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="94"/>
+      <c r="C1" s="88"/>
       <c r="D1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91" t="s">
+      <c r="E1" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="91"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
       <c r="R1" s="6"/>
-      <c r="S1" s="92" t="s">
+      <c r="S1" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="94"/>
+      <c r="T1" s="87"/>
+      <c r="U1" s="87"/>
+      <c r="V1" s="88"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="97"/>
+      <c r="A2" s="91"/>
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1934,11 +1941,11 @@
       <c r="A10" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="88">
+      <c r="B10" s="95">
         <f>SUM(B3:C9)</f>
         <v>16</v>
       </c>
-      <c r="C10" s="88"/>
+      <c r="C10" s="95"/>
       <c r="D10" s="53">
         <f t="shared" ref="D10:V10" si="0">SUM(D3:D9)</f>
         <v>8</v>
@@ -2027,10 +2034,10 @@
       <c r="A11" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="86"/>
+      <c r="C11" s="93"/>
       <c r="D11" s="56" t="s">
         <v>45</v>
       </c>
@@ -2093,10 +2100,10 @@
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="87">
+      <c r="B12" s="94">
         <v>660</v>
       </c>
-      <c r="C12" s="87"/>
+      <c r="C12" s="94"/>
       <c r="D12" s="39">
         <v>705</v>
       </c>
@@ -2159,11 +2166,11 @@
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="89">
+      <c r="B13" s="96">
         <f>ROUNDUP(B10/B12,0)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="89"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="47">
         <f>ROUNDUP(D10/D12,0)</f>
         <v>1</v>
@@ -2245,10 +2252,10 @@
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="90">
+      <c r="B14" s="97">
         <v>9.99</v>
       </c>
-      <c r="C14" s="90"/>
+      <c r="C14" s="97"/>
       <c r="D14" s="49">
         <v>9.99</v>
       </c>
@@ -2311,11 +2318,11 @@
       <c r="A15" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="95">
+      <c r="B15" s="89">
         <f>B14*B13</f>
         <v>9.99</v>
       </c>
-      <c r="C15" s="95"/>
+      <c r="C15" s="89"/>
       <c r="D15" s="40">
         <f>D14*D13</f>
         <v>9.99</v>
@@ -2405,47 +2412,47 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="85"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
       <c r="AC17" s="3"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="85"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
       <c r="M18" s="36"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="85"/>
-      <c r="B19" s="85"/>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="36"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="85"/>
-      <c r="B20" s="85"/>
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="36"/>
@@ -2494,18 +2501,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="12">
+    <mergeCell ref="A17:F20"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:M1"/>
-    <mergeCell ref="A17:F20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:G9 U4 U6 E4:F8 H8 J8:J9 I6:J7 I5:K5 I4:J4 N4:O4 L8:L9 N8 P8:Q8 M5:O5 Q4:R4 Q6:R6 Q5 Q7 M7:O7 N6:O6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Updated BOM with correct power supply price and link
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81D7F8E-516F-4274-979A-8AD029CF1E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650A3532-5949-4DEA-B712-7EED6757F71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38964" yWindow="-3288" windowWidth="34560" windowHeight="19188" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
+    <workbookView xWindow="-44364" yWindow="-3276" windowWidth="34560" windowHeight="19188" xr2:uid="{42FCA7D2-B668-487C-9A6E-A731AE9F01FA}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -698,6 +698,24 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -717,24 +735,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1075,7 +1075,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,14 +1113,14 @@
         <v>73</v>
       </c>
       <c r="B3" s="70">
-        <v>85.99</v>
+        <v>69.989999999999995</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
       </c>
       <c r="D3" s="70">
         <f t="shared" ref="D3:D9" si="0">C3*B3</f>
-        <v>85.99</v>
+        <v>69.989999999999995</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1285,7 +1285,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="70">
-        <f>C15*B15</f>
+        <f t="shared" ref="D15:D20" si="1">C15*B15</f>
         <v>1192</v>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="71">
-        <f>C16*B16</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="71">
-        <f>C17*B17</f>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="71">
-        <f>C18*B18</f>
+        <f t="shared" si="1"/>
         <v>16.309999999999999</v>
       </c>
     </row>
@@ -1345,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="71">
-        <f>C19*B19</f>
+        <f t="shared" si="1"/>
         <v>9.99</v>
       </c>
     </row>
@@ -1360,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="73">
-        <f>C20*B20</f>
+        <f t="shared" si="1"/>
         <v>17.440000000000001</v>
       </c>
     </row>
@@ -1428,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="71">
-        <f t="shared" ref="D25" si="1">C25*B25</f>
+        <f t="shared" ref="D25" si="2">C25*B25</f>
         <v>12.99</v>
       </c>
     </row>
@@ -1454,7 +1454,7 @@
       <c r="B27" s="66"/>
       <c r="D27" s="34">
         <f>SUM(D22:D26,D19:D20,D15:D17,D11:D13,D3:D9)</f>
-        <v>2204.77</v>
+        <v>2188.77</v>
       </c>
       <c r="E27" s="35" t="s">
         <v>72</v>
@@ -1472,7 +1472,7 @@
     <mergeCell ref="A21:D21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="48V 25A 1200W DC Switching Power Supply" xr:uid="{C5468CE6-9D80-4F99-9755-3B3EC496B147}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{C5468CE6-9D80-4F99-9755-3B3EC496B147}"/>
     <hyperlink ref="A4" r:id="rId2" xr:uid="{C48D4976-132F-410B-978C-02AAFE267A50}"/>
     <hyperlink ref="A15" r:id="rId3" xr:uid="{20B0A697-5465-4668-9700-959AE063FEFE}"/>
     <hyperlink ref="A7" r:id="rId4" xr:uid="{5616C467-0CAC-4DB0-AB8B-9CF650AEE797}"/>
@@ -1526,41 +1526,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="90"/>
-      <c r="B1" s="86" t="s">
+      <c r="A1" s="96"/>
+      <c r="B1" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="88"/>
+      <c r="C1" s="94"/>
       <c r="D1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="85" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85" t="s">
+      <c r="E1" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="85"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
       <c r="R1" s="6"/>
-      <c r="S1" s="86" t="s">
+      <c r="S1" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="88"/>
+      <c r="T1" s="93"/>
+      <c r="U1" s="93"/>
+      <c r="V1" s="94"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="91"/>
+      <c r="A2" s="97"/>
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1941,11 +1941,11 @@
       <c r="A10" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="95">
+      <c r="B10" s="88">
         <f>SUM(B3:C9)</f>
         <v>16</v>
       </c>
-      <c r="C10" s="95"/>
+      <c r="C10" s="88"/>
       <c r="D10" s="53">
         <f t="shared" ref="D10:V10" si="0">SUM(D3:D9)</f>
         <v>8</v>
@@ -2034,10 +2034,10 @@
       <c r="A11" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="93"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="56" t="s">
         <v>45</v>
       </c>
@@ -2100,10 +2100,10 @@
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="94">
+      <c r="B12" s="87">
         <v>660</v>
       </c>
-      <c r="C12" s="94"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="39">
         <v>705</v>
       </c>
@@ -2166,11 +2166,11 @@
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="96">
+      <c r="B13" s="89">
         <f>ROUNDUP(B10/B12,0)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="96"/>
+      <c r="C13" s="89"/>
       <c r="D13" s="47">
         <f>ROUNDUP(D10/D12,0)</f>
         <v>1</v>
@@ -2252,10 +2252,10 @@
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="97">
+      <c r="B14" s="90">
         <v>9.99</v>
       </c>
-      <c r="C14" s="97"/>
+      <c r="C14" s="90"/>
       <c r="D14" s="49">
         <v>9.99</v>
       </c>
@@ -2318,11 +2318,11 @@
       <c r="A15" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="89">
+      <c r="B15" s="95">
         <f>B14*B13</f>
         <v>9.99</v>
       </c>
-      <c r="C15" s="89"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="40">
         <f>D14*D13</f>
         <v>9.99</v>
@@ -2412,47 +2412,47 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="92" t="s">
+      <c r="A17" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="92"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
       <c r="AC17" s="3"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
       <c r="M18" s="36"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="92"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="36"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
+      <c r="A20" s="85"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="36"/>
@@ -2501,18 +2501,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="12">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:M1"/>
     <mergeCell ref="A17:F20"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:G9 U4 U6 E4:F8 H8 J8:J9 I6:J7 I5:K5 I4:J4 N4:O4 L8:L9 N8 P8:Q8 M5:O5 Q4:R4 Q6:R6 Q5 Q7 M7:O7 N6:O6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">

</xml_diff>